<commit_message>
Added loads of people to the nucleus list
</commit_message>
<xml_diff>
--- a/customDIctionary.xlsx
+++ b/customDIctionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\claptrap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89B98669-DD85-4DB7-ABB8-41781DBDCB6C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93C403C0-2E5A-4926-A050-F8F2D7571E4B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9375" xr2:uid="{065E9CA2-EFF7-4AAA-8B1A-5CE3FAFF6ACD}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{065E9CA2-EFF7-4AAA-8B1A-5CE3FAFF6ACD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -6557,11 +6557,6 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{03EA1964-9959-4DA9-8B2A-D399BC4B8CF8}" name="Table1" displayName="Table1" ref="A1:BF351" totalsRowShown="0">
   <autoFilter ref="A1:BF351" xr:uid="{DC25ED75-BBD1-453B-9995-DFC1E3E09EA4}">
-    <filterColumn colId="15">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
-    </filterColumn>
     <filterColumn colId="18">
       <filters>
         <filter val="Noun"/>
@@ -6963,9 +6958,9 @@
   <dimension ref="A1:BF351"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomLeft" activeCell="R22" sqref="R22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6988,10 +6983,11 @@
     <col min="16" max="16" width="13.28515625" customWidth="1"/>
     <col min="17" max="17" width="9.140625" style="1"/>
     <col min="18" max="19" width="9.140625" customWidth="1"/>
-    <col min="20" max="22" width="18.42578125" customWidth="1"/>
-    <col min="23" max="26" width="9.140625" customWidth="1"/>
-    <col min="27" max="27" width="9.85546875" customWidth="1"/>
-    <col min="28" max="34" width="9.140625" customWidth="1"/>
+    <col min="20" max="22" width="18.42578125" hidden="1" customWidth="1"/>
+    <col min="23" max="26" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="27" max="27" width="9.85546875" hidden="1" customWidth="1"/>
+    <col min="28" max="31" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="32" max="34" width="9.140625" customWidth="1"/>
     <col min="35" max="37" width="9.28515625" customWidth="1"/>
     <col min="38" max="40" width="9.140625" customWidth="1"/>
     <col min="41" max="43" width="11.5703125" customWidth="1"/>
@@ -7247,7 +7243,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="3" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f t="shared" si="0"/>
         <v>{"spelling": "dad", "group": "_ad", "pos": "Noun", "adult": false, "has": ["a child","kids"], "in": [], "on": [], "from": [], "is": ["a father"], "typeOf": ["a parent"], "supertypeOf": [], "nearlyIs": [], "property": ["paternal","parental"], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -7563,7 +7559,7 @@
         <v>953</v>
       </c>
     </row>
-    <row r="7" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f t="shared" si="0"/>
         <v>{"spelling": "her", "group": "_er", "pos": "Noun", "adult": false, "has": ["a gender"], "in": [], "on": [], "from": ["Venus"], "is": ["a woman"], "typeOf": [], "supertypeOf": ["a girl"], "nearlyIs": [], "property": ["a feminine","a female"], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -7648,7 +7644,7 @@
         <v>1736</v>
       </c>
     </row>
-    <row r="8" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f t="shared" si="0"/>
         <v>{"spelling": "fir", "group": "_er", "pos": "Noun", "adult": false, "has": ["leaves","pinecones","bark"], "in": ["a forest","a wood","the woods"], "on": [], "from": [], "is": [], "typeOf": ["a tree","an evergreen","a pine"], "supertypeOf": [], "nearlyIs": [], "property": ["an evergreen"], "acts": [], "actsCont": [], "recipient": ["chop down"], "recipientPast": []},</v>
@@ -7748,7 +7744,7 @@
         <v>1808</v>
       </c>
     </row>
-    <row r="9" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f t="shared" si="0"/>
         <v>{"spelling": "purr", "group": "_er", "pos": "Noun", "adult": false, "has": [], "in": [], "on": [], "from": ["a cat","a kitten"], "is": ["a meow"], "typeOf": [], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -7824,7 +7820,7 @@
         <v>941</v>
       </c>
     </row>
-    <row r="10" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f t="shared" si="0"/>
         <v>{"spelling": "burr", "group": "_er", "pos": "Noun", "adult": false, "has": ["spikes"], "in": [], "on": [], "from": [], "is": [], "typeOf": [], "supertypeOf": [], "nearlyIs": [], "property": ["a spiky"], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -7897,7 +7893,7 @@
         <v>1655</v>
       </c>
     </row>
-    <row r="11" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f t="shared" si="0"/>
         <v>{"spelling": "sir", "group": "_er", "pos": "Noun", "adult": false, "has": ["a knighthood","a sword","manners"], "in": [], "on": [], "from": [], "is": ["a knight","a gentleman"], "typeOf": ["a man"], "supertypeOf": [], "nearlyIs": [], "property": ["an honorable"], "acts": [], "actsCont": [], "recipient": [], "recipientPast": ["a knighted"]},</v>
@@ -7988,7 +7984,7 @@
         <v>1884</v>
       </c>
     </row>
-    <row r="12" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f t="shared" si="0"/>
         <v>{"spelling": "year", "group": "_er", "pos": "Noun", "adult": false, "has": ["a date","dates","time"], "in": [], "on": [], "from": [], "is": [], "typeOf": [], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -8064,7 +8060,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="13" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
         <f t="shared" si="0"/>
         <v>{"spelling": "cur", "group": "_er", "pos": "Noun", "adult": false, "has": ["a bad attitude","no morals","no breeding"], "in": [], "on": [], "from": [], "is": ["a swine","a scoundrel"], "typeOf": [], "supertypeOf": [], "nearlyIs": ["a dog"], "property": ["a despicable","a mangy"], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -8155,7 +8151,7 @@
         <v>1658</v>
       </c>
     </row>
-    <row r="14" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f t="shared" si="0"/>
         <v>{"spelling": "cat", "group": "_at", "pos": "Noun", "adult": false, "has": ["whiskers","a tail","claws"], "in": [], "on": [], "from": [], "is": ["a feline"], "typeOf": ["a mammal","an animal"], "supertypeOf": ["a kitten","a lion","a tiger"], "nearlyIs": [], "property": ["a feline"], "acts": ["meows","purrs"], "actsCont": ["a meowing","a purring"], "recipient": [], "recipientPast": []},</v>
@@ -8264,7 +8260,7 @@
         <v>1870</v>
       </c>
     </row>
-    <row r="15" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
         <f t="shared" si="0"/>
         <v>{"spelling": "bat", "group": "_at", "pos": "Noun", "adult": false, "has": ["good hearing"], "in": ["a cave"], "on": [], "from": [], "is": [], "typeOf": ["an animal"], "supertypeOf": [], "nearlyIs": ["a vampire"], "property": [], "acts": ["flies"], "actsCont": ["a flying"], "recipient": [], "recipientPast": []},</v>
@@ -8349,7 +8345,7 @@
         <v>1701</v>
       </c>
     </row>
-    <row r="16" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
         <f t="shared" si="0"/>
         <v>{"spelling": "fat", "group": "_at", "pos": "Noun", "adult": false, "has": [], "in": ["a recipe","the kitchen"], "on": [], "from": [], "is": ["grease"], "typeOf": ["an ingredient"], "supertypeOf": ["lard","butter"], "nearlyIs": ["oil"], "property": ["a greasy"], "acts": [], "actsCont": [], "recipient": ["cook with"], "recipientPast": ["a cooked with"]},</v>
@@ -8446,7 +8442,7 @@
         <v>1885</v>
       </c>
     </row>
-    <row r="17" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
         <f t="shared" si="0"/>
         <v>{"spelling": "hat", "group": "_at", "pos": "Noun", "adult": false, "has": ["a brim"], "in": [], "on": ["a head","your head"], "from": [], "is": [], "typeOf": ["clothing","headgear"], "supertypeOf": ["a cap","a beanie","a beret"], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": ["wear"], "recipientPast": ["a worn"]},</v>
@@ -8543,7 +8539,7 @@
         <v>1886</v>
       </c>
     </row>
-    <row r="18" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
         <f t="shared" si="0"/>
         <v>{"spelling": "that", "group": "_at", "pos": "Noun", "adult": false, "has": [], "in": [], "on": [], "from": [], "is": [], "typeOf": [], "supertypeOf": [], "nearlyIs": ["a thing","an item","an object"], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -8619,7 +8615,7 @@
         <v>982</v>
       </c>
     </row>
-    <row r="19" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
         <f t="shared" si="0"/>
         <v>{"spelling": "pat", "group": "_at", "pos": "Noun", "adult": false, "has": [], "in": [], "on": [], "from": [], "is": [], "typeOf": ["a touch"], "supertypeOf": [], "nearlyIs": ["a fondle"], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -8692,10 +8688,10 @@
         <v>969</v>
       </c>
     </row>
-    <row r="20" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
         <f t="shared" si="0"/>
-        <v>{"spelling": "prat", "group": "_at", "pos": "Noun", "adult": true, "has": ["no brains","bad ideas"], "in": [], "on": [], "from": [], "is": ["an idiot","a moron","a jackass"], "typeOf": [], "supertypeOf": [], "nearlyIs": [], "property": ["an idiotic","a stupid","an annoying"], "acts": ["acts stupid","says stupid things"], "actsCont": [], "recipient": [], "recipientPast": []},</v>
+        <v>{"spelling": "prat", "group": "_at", "pos": "Noun", "adult": false, "has": ["no brains","bad ideas"], "in": [], "on": [], "from": [], "is": ["an idiot","a moron","a jackass"], "typeOf": [], "supertypeOf": [], "nearlyIs": [], "property": ["an idiotic","a stupid","an annoying"], "acts": ["acts stupid","says stupid things"], "actsCont": [], "recipient": [], "recipientPast": []},</v>
       </c>
       <c r="B20" t="str">
         <f t="shared" si="1"/>
@@ -8755,9 +8751,6 @@
       <c r="Q20" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="R20" t="b">
-        <v>1</v>
-      </c>
       <c r="S20" t="s">
         <v>217</v>
       </c>
@@ -8792,7 +8785,7 @@
         <v>1815</v>
       </c>
     </row>
-    <row r="21" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
         <f t="shared" si="0"/>
         <v>{"spelling": "at", "group": "_at", "pos": "Noun", "adult": false, "has": [], "in": [], "on": [], "from": [], "is": [], "typeOf": [], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -8859,7 +8852,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="22" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
         <f t="shared" si="0"/>
         <v>{"spelling": "spat", "group": "_at", "pos": "Noun", "adult": false, "has": [], "in": [], "on": [], "from": [], "is": ["a domestic"], "typeOf": ["a fight","an argument"], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -9005,7 +8998,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="24" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
         <f t="shared" si="0"/>
         <v>{"spelling": "vat", "group": "_at", "pos": "Noun", "adult": false, "has": ["a lot in it"], "in": [], "on": [], "from": [], "is": [], "typeOf": ["a container","a lot"], "supertypeOf": [], "nearlyIs": ["a pan"], "property": ["a large","a huge"], "acts": [], "actsCont": [], "recipient": ["fill"], "recipientPast": ["a filled"]},</v>
@@ -9096,7 +9089,7 @@
         <v>1887</v>
       </c>
     </row>
-    <row r="25" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
         <f>CONCATENATE("{""spelling"": """,Q25,""", ""group"": """,O25,""", ""pos"": """,S25,""", ""adult"": ",IF(R25=TRUE,"true","false"),", ""has"": [",B25,"]",", ""in"": [",C25,"]",", ""on"": [",D25,"]",", ""from"": [",E25,"]",", ""is"": [",F25,"]",", ""typeOf"": [",G25,"]",", ""supertypeOf"": [",H25,"]",", ""nearlyIs"": [",I25,"]",", ""property"": [",J25,"]",", ""acts"": [",K25,"]",", ""actsCont"": [",L25,"]",", ""recipient"": [",M25,"]",", ""recipientPast"": [",N25,"]},")</f>
         <v>{"spelling": "mat", "group": "_at", "pos": "Noun", "adult": false, "has": [], "in": ["front of a door"], "on": [], "from": [], "is": [], "typeOf": ["furniture"], "supertypeOf": [], "nearlyIs": ["a rug"], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -9172,7 +9165,7 @@
         <v>986</v>
       </c>
     </row>
-    <row r="26" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
         <f t="shared" si="0"/>
         <v>{"spelling": "gnat", "group": "_at", "pos": "Noun", "adult": false, "has": ["wings"], "in": [], "on": ["your leg"], "from": [], "is": [], "typeOf": ["a fly","an insect"], "supertypeOf": ["a midgey","a mosquito"], "nearlyIs": [], "property": [], "acts": ["flies"], "actsCont": ["a flying"], "recipient": ["swat"], "recipientPast": []},</v>
@@ -9266,7 +9259,7 @@
         <v>1817</v>
       </c>
     </row>
-    <row r="27" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
         <f t="shared" si="0"/>
         <v>{"spelling": "twat", "group": "_at", "pos": "Noun", "adult": true, "has": ["labia","bad ideas","a clitoris"], "in": [], "on": [], "from": [], "is": ["an idiot","a moron","a jackass"], "typeOf": ["genitalia","a body part"], "supertypeOf": [], "nearlyIs": ["a pussy","a vagina"], "property": [], "acts": [], "actsCont": [], "recipient": ["fuck"], "recipientPast": ["a fucked"]},</v>
@@ -9372,7 +9365,7 @@
         <v>1888</v>
       </c>
     </row>
-    <row r="28" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
         <f t="shared" si="0"/>
         <v>{"spelling": "con", "group": "_on", "pos": "Noun", "adult": false, "has": ["people confused","a jail sentence"], "in": ["jail","prison"], "on": [], "from": ["prison","jail"], "is": ["a scoundrel","a prisoner"], "typeOf": ["a criminal","a liar"], "supertypeOf": [], "nearlyIs": [], "property": ["a deceitful","a criminal"], "acts": ["lies","schemes"], "actsCont": ["a lying","a scheming"], "recipient": ["imprison","jail"], "recipientPast": ["an imprisoned","a jailed"]},</v>
@@ -9569,7 +9562,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="30" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
         <f t="shared" si="0"/>
         <v>{"spelling": "don", "group": "_on", "pos": "Noun", "adult": false, "has": ["mafiosos","a horses head","hired goons"], "in": ["the mafia"], "on": [], "from": ["the mafia"], "is": ["a crime lord","a king pin","a mob boss"], "typeOf": ["a criminal","a mafioso","a gang member"], "supertypeOf": [], "nearlyIs": [], "property": ["a criminal"], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -9672,7 +9665,7 @@
         <v>993</v>
       </c>
     </row>
-    <row r="31" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A31" t="str">
         <f t="shared" si="0"/>
         <v>{"spelling": "none", "group": "_on", "pos": "Noun", "adult": false, "has": ["nothing","nobody"], "in": [], "on": [], "from": [], "is": ["nothing"], "typeOf": ["an amount"], "supertypeOf": [], "nearlyIs": ["an emptyness","an absence","a lack"], "property": ["an empty"], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -9763,7 +9756,7 @@
         <v>1666</v>
       </c>
     </row>
-    <row r="32" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A32" t="str">
         <f t="shared" si="0"/>
         <v>{"spelling": "one", "group": "_on", "pos": "Noun", "adult": false, "has": [], "in": [], "on": [], "from": [], "is": ["a single"], "typeOf": ["a number","a digit"], "supertypeOf": [], "nearlyIs": [], "property": ["a single"], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -9842,7 +9835,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="33" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A33" t="str">
         <f t="shared" si="0"/>
         <v>{"spelling": "son", "group": "_un", "pos": "Noun", "adult": false, "has": ["parents"], "in": [], "on": [], "from": [], "is": [], "typeOf": ["a child","a kid"], "supertypeOf": [], "nearlyIs": ["a firstborn"], "property": ["a male"], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -9924,7 +9917,7 @@
         <v>1667</v>
       </c>
     </row>
-    <row r="34" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A34" t="str">
         <f t="shared" si="0"/>
         <v>{"spelling": "net", "group": "_et", "pos": "Noun", "adult": false, "has": ["fish in it"], "in": ["the ocean","the sea","a river"], "on": [], "from": [], "is": [], "typeOf": ["a tool"], "supertypeOf": ["a web"], "nearlyIs": [], "property": [], "acts": ["catches fish"], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -10012,7 +10005,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="35" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A35" t="str">
         <f t="shared" si="0"/>
         <v>{"spelling": "pet", "group": "_et", "pos": "Noun", "adult": false, "has": ["an owner","a tail"], "in": ["a kennel"], "on": ["your sofa"], "from": ["the pound"], "is": [], "typeOf": ["an animal"], "supertypeOf": ["a cat","a dog","a goldfish"], "nearlyIs": [], "property": ["a fluffy","a canine","a feline"], "acts": ["meows","barks","purrs"], "actsCont": ["a meowing","a purring","barking"], "recipient": ["play with","feed","walk"], "recipientPast": []},</v>
@@ -10142,7 +10135,7 @@
         <v>1826</v>
       </c>
     </row>
-    <row r="36" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A36" t="str">
         <f t="shared" si="0"/>
         <v>{"spelling": "set", "group": "_et", "pos": "Noun", "adult": false, "has": [], "in": [], "on": [], "from": [], "is": ["a group"], "typeOf": ["a collection"], "supertypeOf": [], "nearlyIs": ["a list"], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -10218,7 +10211,7 @@
         <v>1013</v>
       </c>
     </row>
-    <row r="37" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A37" t="str">
         <f t="shared" si="0"/>
         <v>{"spelling": "vet", "group": "_et", "pos": "Noun", "adult": false, "has": ["animals","tiny bandages","medical training"], "in": ["a clinic"], "on": [], "from": [], "is": [], "typeOf": ["a clinician","a medical proffesional"], "supertypeOf": ["a horse doctor"], "nearlyIs": ["a doctor"], "property": [], "acts": ["treats animals"], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -10312,7 +10305,7 @@
         <v>1827</v>
       </c>
     </row>
-    <row r="38" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A38" t="str">
         <f t="shared" si="0"/>
         <v>{"spelling": "bet", "group": "_et", "pos": "Noun", "adult": false, "has": ["money on it","a risk","a chance of winning"], "in": ["a casino","a racecourse"], "on": [], "from": [], "is": ["a stake","a gamble"], "typeOf": [], "supertypeOf": [], "nearlyIs": ["a risk","a chance"], "property": [], "acts": [], "actsCont": [], "recipient": ["place"], "recipientPast": []},</v>
@@ -10409,10 +10402,10 @@
         <v>1828</v>
       </c>
     </row>
-    <row r="39" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A39" t="str">
         <f t="shared" si="0"/>
-        <v>{"spelling": "jay", "group": "_et", "pos": "Noun", "adult": false, "has": ["a beak","a nest"], "in": ["a tree","the sky"], "on": [], "from": [], "is": [], "typeOf": ["a bird","an animal"], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": ["flies","caws"], "actsCont": ["a flying","a cawing"], "recipient": [], "recipientPast": []},</v>
+        <v>{"spelling": "jay", "group": "_ay", "pos": "Noun", "adult": false, "has": ["a beak","a nest"], "in": ["a tree","the sky"], "on": [], "from": [], "is": [], "typeOf": ["a bird","an animal"], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": ["flies","caws"], "actsCont": ["a flying","a cawing"], "recipient": [], "recipientPast": []},</v>
       </c>
       <c r="B39" t="str">
         <f t="shared" si="1"/>
@@ -10467,7 +10460,7 @@
         <v/>
       </c>
       <c r="O39" t="s">
-        <v>32</v>
+        <v>173</v>
       </c>
       <c r="Q39" s="1" t="s">
         <v>255</v>
@@ -10506,7 +10499,7 @@
         <v>1873</v>
       </c>
     </row>
-    <row r="40" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A40" t="str">
         <f t="shared" si="0"/>
         <v>{"spelling": "kit", "group": "_it", "pos": "Noun", "adult": false, "has": [], "in": [], "on": [], "from": [], "is": [], "typeOf": ["equipment"], "supertypeOf": [], "nearlyIs": ["a toolbox"], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -10579,7 +10572,7 @@
         <v>799</v>
       </c>
     </row>
-    <row r="41" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A41" t="str">
         <f t="shared" si="0"/>
         <v>{"spelling": "wit", "group": "_it", "pos": "Noun", "adult": false, "has": ["funny ideas","good conversation"], "in": [], "on": ["a panel show","stage"], "from": [], "is": ["a comedian"], "typeOf": ["a writer","an author"], "supertypeOf": [], "nearlyIs": ["a joker"], "property": ["an intelligent","a funny","a smart"], "acts": ["jokes"], "actsCont": ["a joking"], "recipient": [], "recipientPast": []},</v>
@@ -10685,7 +10678,7 @@
         <v>1874</v>
       </c>
     </row>
-    <row r="42" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A42" t="str">
         <f t="shared" si="0"/>
         <v>{"spelling": "writ", "group": "_it", "pos": "Noun", "adult": false, "has": ["a signature","legal groundings"], "in": ["a court","a courtroom"], "on": [], "from": [], "is": [], "typeOf": ["a court order"], "supertypeOf": ["a summons","a subpoena"], "nearlyIs": [], "property": ["a legal"], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -10776,7 +10769,7 @@
         <v>1672</v>
       </c>
     </row>
-    <row r="43" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A43" t="str">
         <f t="shared" si="0"/>
         <v>{"spelling": "tit", "group": "_it", "pos": "Noun", "adult": true, "has": ["a nipple","a bra"], "in": ["a bra"], "on": ["your chest"], "from": [], "is": ["a breast","a boob"], "typeOf": ["genitalia","a body part"], "supertypeOf": [], "nearlyIs": [], "property": ["a perky"], "acts": ["lactates","jiggles"], "actsCont": ["a lactating","a jiggling"], "recipient": [], "recipientPast": []},</v>
@@ -10885,7 +10878,7 @@
         <v>1876</v>
       </c>
     </row>
-    <row r="44" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A44" t="str">
         <f t="shared" si="0"/>
         <v>{"spelling": "pit", "group": "_it", "pos": "Noun", "adult": false, "has": ["spikes in it"], "in": ["a date","an olive"], "on": ["the ground"], "from": [], "is": [], "typeOf": ["a hole","a trap"], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": ["fall in to"], "recipientPast": []},</v>
@@ -10973,7 +10966,7 @@
         <v>1840</v>
       </c>
     </row>
-    <row r="45" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A45" t="str">
         <f t="shared" si="0"/>
         <v>{"spelling": "it", "group": "_it", "pos": "Noun", "adult": false, "has": [], "in": [], "on": [], "from": [], "is": [], "typeOf": [], "supertypeOf": [], "nearlyIs": ["a thing","an item","an object"], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -11049,7 +11042,7 @@
         <v>982</v>
       </c>
     </row>
-    <row r="46" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A46" t="str">
         <f t="shared" si="0"/>
         <v>{"spelling": "fit", "group": "_it", "pos": "Noun", "adult": false, "has": [], "in": [], "on": [], "from": [], "is": [], "typeOf": [], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -11116,7 +11109,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="47" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A47" t="str">
         <f t="shared" si="0"/>
         <v>{"spelling": "git", "group": "_it", "pos": "Noun", "adult": true, "has": ["no friends","a bad attitude"], "in": [], "on": [], "from": [], "is": [], "typeOf": [], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -11192,7 +11185,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="48" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A48" t="str">
         <f t="shared" si="0"/>
         <v>{"spelling": "hit", "group": "_it", "pos": "Noun", "adult": false, "has": [], "in": [], "on": ["target"], "from": ["a good shot"], "is": [], "typeOf": ["a success","a collision"], "supertypeOf": [], "nearlyIs": [], "property": ["a successful"], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -11274,7 +11267,7 @@
         <v>1674</v>
       </c>
     </row>
-    <row r="49" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A49" t="str">
         <f t="shared" si="0"/>
         <v>{"spelling": "zit", "group": "_it", "pos": "Noun", "adult": false, "has": ["pus"], "in": [], "on": ["a teenager","your face","your chin"], "from": [], "is": ["a pimple"], "typeOf": ["a spot","a blemish"], "supertypeOf": [], "nearlyIs": ["a wart","a mole"], "property": ["a spotty"], "acts": [], "actsCont": [], "recipient": ["pop"], "recipientPast": ["a popped"]},</v>
@@ -11377,7 +11370,7 @@
         <v>1891</v>
       </c>
     </row>
-    <row r="50" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A50" t="str">
         <f t="shared" si="0"/>
         <v>{"spelling": "Brit", "group": "_it", "pos": "Noun", "adult": false, "has": ["a drinking problem","bad teeth","a great accent"], "in": ["England","the UK","Britain"], "on": [], "from": ["England","the UK","Britain"], "is": [], "typeOf": ["a European"], "supertypeOf": ["an Englishman","a Scotsman","a Welshman"], "nearlyIs": [], "property": ["an English"], "acts": ["drinks tea","talks about the weather","queues"], "actsCont": ["a queuing"], "recipient": [], "recipientPast": []},</v>
@@ -11498,7 +11491,7 @@
         <v>1877</v>
       </c>
     </row>
-    <row r="51" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A51" t="str">
         <f t="shared" si="0"/>
         <v>{"spelling": "twit", "group": "_it", "pos": "Noun", "adult": true, "has": ["bad ideas"], "in": [], "on": [], "from": [], "is": ["an idiot","a moron","a jackass"], "typeOf": [], "supertypeOf": [], "nearlyIs": [], "property": ["an idiotic","a stupid","an annoying"], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -11589,7 +11582,7 @@
         <v>1662</v>
       </c>
     </row>
-    <row r="52" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A52" t="str">
         <f t="shared" si="0"/>
         <v>{"spelling": "nit", "group": "_it", "pos": "Noun", "adult": false, "has": [], "in": ["your hair","your head"], "on": ["a kid's head"], "from": [], "is": [], "typeOf": ["an insect","a pest","a hair problem"], "supertypeOf": [], "nearlyIs": [], "property": ["an itchy"], "acts": [], "actsCont": [], "recipient": ["scratch"], "recipientPast": []},</v>
@@ -11680,7 +11673,7 @@
         <v>1843</v>
       </c>
     </row>
-    <row r="53" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A53" t="str">
         <f t="shared" si="0"/>
         <v>{"spelling": "mit", "group": "_it", "pos": "Noun", "adult": false, "has": ["fingers"], "in": [], "on": ["your hand"], "from": [], "is": [], "typeOf": ["a hand","a glove"], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -11759,7 +11752,7 @@
         <v>1045</v>
       </c>
     </row>
-    <row r="54" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A54" t="str">
         <f t="shared" si="0"/>
         <v>{"spelling": "shit", "group": "_it", "pos": "Noun", "adult": true, "has": ["a bad smell","a bit of sweetcorn in it"], "in": ["the toilet"], "on": ["the bottom of your shoe"], "from": ["an arse"], "is": ["a turd","a crap","faeces"], "typeOf": ["a dump","a floater","a bodily function"], "supertypeOf": ["diarrhea"], "nearlyIs": ["rubbish","junk"], "property": ["a smelly"], "acts": ["stinks","smells"], "actsCont": ["a stinking"], "recipient": ["flush"], "recipientPast": ["a flushed"]},</v>
@@ -11889,7 +11882,7 @@
         <v>1892</v>
       </c>
     </row>
-    <row r="55" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A55" t="str">
         <f t="shared" si="0"/>
         <v>{"spelling": "chit", "group": "_it", "pos": "Noun", "adult": false, "has": ["a signature"], "in": [], "on": [], "from": [], "is": [], "typeOf": [], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": ["write"], "recipientPast": ["a written"]},</v>
@@ -11965,7 +11958,7 @@
         <v>1682</v>
       </c>
     </row>
-    <row r="56" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A56" t="str">
         <f t="shared" si="0"/>
         <v>{"spelling": "spit", "group": "_it", "pos": "Noun", "adult": false, "has": [], "in": ["your mouth"], "on": [], "from": ["your mouth"], "is": [], "typeOf": ["an emission","a bodily function"], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -12044,7 +12037,7 @@
         <v>1055</v>
       </c>
     </row>
-    <row r="57" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A57" t="str">
         <f t="shared" si="0"/>
         <v>{"spelling": "skit", "group": "_it", "pos": "Noun", "adult": false, "has": ["comedians in it","an audience"], "in": [], "on": ["stage","tv"], "from": [], "is": [], "typeOf": ["a sketch","a parody"], "supertypeOf": [], "nearlyIs": ["a joke"], "property": ["a funny","a hilarious"], "acts": [], "actsCont": [], "recipient": ["perform"], "recipientPast": ["a performed"]},</v>
@@ -12214,7 +12207,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="59" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A59" t="str">
         <f t="shared" si="14"/>
         <v>{"spelling": "watt", "group": "_ot", "pos": "Noun", "adult": false, "has": ["power"], "in": ["a circuit","a wire"], "on": [], "from": ["a generator"], "is": [], "typeOf": ["a measurement","a unit"], "supertypeOf": [], "nearlyIs": [], "property": ["an electrical"], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -12302,7 +12295,7 @@
         <v>1773</v>
       </c>
     </row>
-    <row r="60" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A60" t="str">
         <f t="shared" si="14"/>
         <v>{"spelling": "tot", "group": "_ot", "pos": "Noun", "adult": false, "has": ["parents","a diaper","a dummy"], "in": ["diapers","school","kindergarten"], "on": [], "from": [], "is": ["a child","a kid","a youth"], "typeOf": ["a person"], "supertypeOf": ["a baby","a toddler","an urchin"], "nearlyIs": [], "property": ["a young"], "acts": ["cries"], "actsCont": ["a crying"], "recipient": ["change","feed","burp"], "recipientPast": []},</v>
@@ -12426,7 +12419,7 @@
         <v>2070</v>
       </c>
     </row>
-    <row r="61" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A61" t="str">
         <f t="shared" si="14"/>
         <v>{"spelling": "yacht", "group": "_ot", "pos": "Noun", "adult": false, "has": ["sails","a mast","a skipper"], "in": ["port"], "on": ["the seas","a lake"], "from": [], "is": [], "typeOf": ["a boat","a ship","a vehicle"], "supertypeOf": [], "nearlyIs": ["a sailboat"], "property": [], "acts": ["sails"], "actsCont": ["a sailing"], "recipient": ["sail","board"], "recipientPast": ["a sailed"]},</v>
@@ -12538,7 +12531,7 @@
         <v>2072</v>
       </c>
     </row>
-    <row r="62" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A62" t="str">
         <f t="shared" si="14"/>
         <v>{"spelling": "pot", "group": "_ot", "pos": "Noun", "adult": true, "has": ["a lid","a handle"], "in": ["a kitchen","a bong","a joint"], "on": [], "from": [], "is": ["weed","marijuana"], "typeOf": ["a drug"], "supertypeOf": ["a joint"], "nearlyIs": ["a pan"], "property": [], "acts": [], "actsCont": [], "recipient": ["smoke","cook with","toke"], "recipientPast": []},</v>
@@ -12647,7 +12640,7 @@
         <v>2074</v>
       </c>
     </row>
-    <row r="63" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A63" t="str">
         <f t="shared" si="14"/>
         <v>{"spelling": "plot", "group": "_ot", "pos": "Noun", "adult": false, "has": ["conspirators"], "in": [], "on": [], "from": [], "is": [], "typeOf": ["a plan"], "supertypeOf": ["a scheme"], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -12793,7 +12786,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="65" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A65" t="str">
         <f t="shared" si="14"/>
         <v>{"spelling": "snot", "group": "_ot", "pos": "Noun", "adult": false, "has": [], "in": ["a nostril","a tissue","a nose"], "on": [], "from": ["a nose","a nostril"], "is": [], "typeOf": ["an emission"], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": ["sneeze"], "recipientPast": ["a sneezed"]},</v>
@@ -12884,7 +12877,7 @@
         <v>2076</v>
       </c>
     </row>
-    <row r="66" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A66" t="str">
         <f t="shared" si="14"/>
         <v>{"spelling": "spot", "group": "_ot", "pos": "Noun", "adult": false, "has": ["pus"], "in": [], "on": ["a teenager","your face","your chin"], "from": [], "is": [], "typeOf": ["a blemish"], "supertypeOf": ["a pimple","a zit"], "nearlyIs": ["a wart","a mole"], "property": ["a round"], "acts": [], "actsCont": [], "recipient": ["pop"], "recipientPast": ["a popped"]},</v>
@@ -12987,7 +12980,7 @@
         <v>1891</v>
       </c>
     </row>
-    <row r="67" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A67" t="str">
         <f t="shared" si="14"/>
         <v>{"spelling": "dot", "group": "_ot", "pos": "Noun", "adult": false, "has": [], "in": [], "on": [], "from": [], "is": ["a spot"], "typeOf": ["a mark"], "supertypeOf": [], "nearlyIs": [], "property": ["a round"], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -13063,7 +13056,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="68" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A68" t="str">
         <f t="shared" si="14"/>
         <v>{"spelling": "lot", "group": "_ot", "pos": "Noun", "adult": false, "has": [], "in": [], "on": [], "from": [], "is": ["a load","masses"], "typeOf": [], "supertypeOf": [], "nearlyIs": [], "property": ["an abundant"], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -13139,7 +13132,7 @@
         <v>1775</v>
       </c>
     </row>
-    <row r="69" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A69" t="str">
         <f t="shared" si="14"/>
         <v>{"spelling": "cot", "group": "_ot", "pos": "Noun", "adult": false, "has": ["a pillow","a blanker"], "in": ["a bedroom","a jail cell","a prison cell"], "on": [], "from": [], "is": [], "typeOf": ["a bed"], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -13224,7 +13217,7 @@
         <v>1456</v>
       </c>
     </row>
-    <row r="70" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A70" t="str">
         <f t="shared" si="14"/>
         <v>{"spelling": "bait", "group": "_ate", "pos": "Noun", "adult": false, "has": [], "in": ["a trap"], "on": ["a fishing hook","a hook"], "from": [], "is": [], "typeOf": [], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -13300,7 +13293,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="71" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A71" t="str">
         <f t="shared" si="14"/>
         <v>{"spelling": "date", "group": "_ate", "pos": "Noun", "adult": false, "has": ["a pit"], "in": [], "on": ["valentine's day","a tree"], "from": [], "is": [], "typeOf": ["a time period","a fruit"], "supertypeOf": [], "nearlyIs": ["a prune"], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -13385,7 +13378,7 @@
         <v>1087</v>
       </c>
     </row>
-    <row r="72" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A72" t="str">
         <f t="shared" si="14"/>
         <v>{"spelling": "fate", "group": "_ate", "pos": "Noun", "adult": false, "has": [], "in": [], "on": [], "from": [], "is": ["an outcome"], "typeOf": [], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -13455,7 +13448,7 @@
         <v>1089</v>
       </c>
     </row>
-    <row r="73" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A73" t="str">
         <f t="shared" si="14"/>
         <v>{"spelling": "gait", "group": "_ate", "pos": "Noun", "adult": false, "has": ["a funny way of walking","taken steps"], "in": [], "on": [], "from": [], "is": ["a walk"], "typeOf": ["a movement"], "supertypeOf": [], "nearlyIs": ["a step"], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -13537,7 +13530,7 @@
         <v>1092</v>
       </c>
     </row>
-    <row r="74" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A74" t="str">
         <f t="shared" si="14"/>
         <v>{"spelling": "gate", "group": "_ate", "pos": "Noun", "adult": false, "has": ["a handle","a fence"], "in": ["a fence"], "on": [], "from": [], "is": [], "typeOf": ["an entrance","a door"], "supertypeOf": ["a portcullis"], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": ["open","close"], "recipientPast": ["an opened","a closed"]},</v>
@@ -13634,7 +13627,7 @@
         <v>1787</v>
       </c>
     </row>
-    <row r="75" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A75" t="str">
         <f t="shared" si="14"/>
         <v>{"spelling": "wait", "group": "_ate", "pos": "Noun", "adult": false, "has": ["a pause","time"], "in": [], "on": [], "from": [], "is": ["a pause"], "typeOf": [], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -13710,7 +13703,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="76" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A76" t="str">
         <f t="shared" si="14"/>
         <v>{"spelling": "mate", "group": "_ate", "pos": "Noun", "adult": false, "has": ["friends","a friend","pals"], "in": [], "on": [], "from": [], "is": ["a friend","a pal","a buddy"], "typeOf": [], "supertypeOf": ["a BFF"], "nearlyIs": ["an aquaintance"], "property": ["a friendly"], "acts": [], "actsCont": [], "recipient": ["befriend"], "recipientPast": ["a befriended"]},</v>
@@ -13810,7 +13803,7 @@
         <v>1898</v>
       </c>
     </row>
-    <row r="77" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A77" t="str">
         <f t="shared" si="14"/>
         <v>{"spelling": "state", "group": "_ate", "pos": "Noun", "adult": false, "has": ["a capital"], "in": [], "on": [], "from": [], "is": [], "typeOf": ["a region","an area","a place"], "supertypeOf": [], "nearlyIs": ["a situation","a case"], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -13895,7 +13888,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="78" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A78" t="str">
         <f t="shared" si="14"/>
         <v>{"spelling": "art", "group": "_art", "pos": "Noun", "adult": false, "has": ["brush strokes","a frame"], "in": ["a gallery"], "on": ["the wall"], "from": ["a gallery","a painter","an artist"], "is": ["a decoration"], "typeOf": [], "supertypeOf": ["a painting","a statue","a mural"], "nearlyIs": [], "property": ["a decorative","a beautiful"], "acts": [], "actsCont": [], "recipient": ["paint","draw","sculpt"], "recipientPast": ["a painted","a drawn","a sculpted"]},</v>
@@ -14019,7 +14012,7 @@
         <v>1901</v>
       </c>
     </row>
-    <row r="79" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A79" t="str">
         <f t="shared" si="14"/>
         <v>{"spelling": "tart", "group": "_art", "pos": "Noun", "adult": false, "has": ["a filling","pastry"], "in": [], "on": [], "from": ["a baker"], "is": [], "typeOf": ["a cake","a dessert"], "supertypeOf": [], "nearlyIs": ["a pie"], "property": ["a delicious"], "acts": [], "actsCont": [], "recipient": ["eat","bake"], "recipientPast": ["a baked"]},</v>
@@ -14116,7 +14109,7 @@
         <v>1902</v>
       </c>
     </row>
-    <row r="80" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A80" t="str">
         <f t="shared" si="14"/>
         <v>{"spelling": "part", "group": "_art", "pos": "Noun", "adult": false, "has": [], "in": [], "on": [], "from": [], "is": ["a section","a component","a segment"], "typeOf": [], "supertypeOf": ["a half","a quarter"], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -14198,7 +14191,7 @@
         <v>1116</v>
       </c>
     </row>
-    <row r="81" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A81" t="str">
         <f t="shared" si="14"/>
         <v>{"spelling": "dart", "group": "_art", "pos": "Noun", "adult": false, "has": ["a board","fins","a tip"], "in": [], "on": ["a dartboard"], "from": [], "is": [], "typeOf": [], "supertypeOf": [], "nearlyIs": [], "property": ["a pointy"], "acts": [], "actsCont": [], "recipient": ["throw"], "recipientPast": ["a thrown"]},</v>
@@ -14286,7 +14279,7 @@
         <v>1903</v>
       </c>
     </row>
-    <row r="82" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A82" t="str">
         <f t="shared" si="14"/>
         <v>{"spelling": "fart", "group": "_art", "pos": "Noun", "adult": true, "has": ["a smell","a bad smell"], "in": [], "on": [], "from": ["an arse","a lot of beans"], "is": [], "typeOf": ["a gas","wind","a stench"], "supertypeOf": [], "nearlyIs": [], "property": ["a smelly"], "acts": ["stinks","smells"], "actsCont": ["a stinking"], "recipient": [], "recipientPast": []},</v>
@@ -14389,7 +14382,7 @@
         <v>1878</v>
       </c>
     </row>
-    <row r="83" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A83" t="str">
         <f t="shared" si="14"/>
         <v>{"spelling": "heart", "group": "_art", "pos": "Noun", "adult": false, "has": ["blood","ventricles"], "in": ["your torso","your chest"], "on": [], "from": [], "is": [], "typeOf": ["an organ","a shape"], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": ["beats"], "actsCont": ["a beating"], "recipient": [], "recipientPast": []},</v>
@@ -14480,7 +14473,7 @@
         <v>1882</v>
       </c>
     </row>
-    <row r="84" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A84" t="str">
         <f t="shared" si="14"/>
         <v>{"spelling": "shart", "group": "_art", "pos": "Noun", "adult": true, "has": ["a smell","a bad smell","a stain"], "in": ["your trousers"], "on": [], "from": ["an arse","a curry","mexican food"], "is": [], "typeOf": ["an accident"], "supertypeOf": [], "nearlyIs": [], "property": ["a smelly"], "acts": ["stinks","smells","stains"], "actsCont": ["a stinking","a staining"], "recipient": ["clean up"], "recipientPast": []},</v>
@@ -14595,7 +14588,7 @@
         <v>1945</v>
       </c>
     </row>
-    <row r="85" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A85" t="str">
         <f t="shared" si="14"/>
         <v>{"spelling": "mart", "group": "_art", "pos": "Noun", "adult": false, "has": ["a shopkeeper","goods"], "in": [], "on": [], "from": [], "is": [], "typeOf": ["a shop","a store"], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": ["shop at","buy from"], "recipientPast": []},</v>
@@ -14680,7 +14673,7 @@
         <v>1867</v>
       </c>
     </row>
-    <row r="86" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A86" t="str">
         <f t="shared" si="14"/>
         <v>{"spelling": "start", "group": "_art", "pos": "Noun", "adult": false, "has": [], "in": ["the beginning"], "on": [], "from": ["the beginning"], "is": ["a beginning"], "typeOf": [], "supertypeOf": [], "nearlyIs": ["an opening"], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -14759,7 +14752,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="87" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A87" t="str">
         <f t="shared" si="14"/>
         <v>{"spelling": "woe", "group": "_o", "pos": "Noun", "adult": false, "has": ["depression","tears"], "in": [], "on": [], "from": [], "is": [], "typeOf": ["a problem"], "supertypeOf": [], "nearlyIs": [], "property": ["a depressing","a sad"], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -14841,7 +14834,7 @@
         <v>1690</v>
       </c>
     </row>
-    <row r="88" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A88" t="str">
         <f t="shared" si="14"/>
         <v>{"spelling": "roe", "group": "_o", "pos": "Noun", "adult": false, "has": ["eggs","a fishy smell"], "in": [], "on": [], "from": ["a fish"], "is": ["fish eggs"], "typeOf": ["seafood","eggs"], "supertypeOf": [], "nearlyIs": [], "property": ["a fishy"], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -14929,7 +14922,7 @@
         <v>1691</v>
       </c>
     </row>
-    <row r="89" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A89" t="str">
         <f t="shared" si="14"/>
         <v>{"spelling": "toe", "group": "_o", "pos": "Noun", "adult": false, "has": ["a nail"], "in": ["a shoe"], "on": ["a foot"], "from": [], "is": [], "typeOf": ["a body part"], "supertypeOf": [], "nearlyIs": ["a finger"], "property": [], "acts": [], "actsCont": [], "recipient": ["stub"], "recipientPast": ["a stubbed"]},</v>
@@ -15017,7 +15010,7 @@
         <v>1904</v>
       </c>
     </row>
-    <row r="90" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A90" t="str">
         <f t="shared" si="14"/>
         <v>{"spelling": "doe", "group": "_o", "pos": "Noun", "adult": false, "has": ["hooves"], "in": [], "on": [], "from": [], "is": ["a female deer"], "typeOf": ["a deer","an animal","a mammal"], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -15099,7 +15092,7 @@
         <v>957</v>
       </c>
     </row>
-    <row r="91" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A91" t="str">
         <f t="shared" si="14"/>
         <v>{"spelling": "dough", "group": "_o", "pos": "Noun", "adult": false, "has": ["yeast","flour"], "in": ["a bakery"], "on": [], "from": ["a baker"], "is": [], "typeOf": ["an ingredient"], "supertypeOf": [], "nearlyIs": ["a batter"], "property": [], "acts": [], "actsCont": [], "recipient": ["knead","bake"], "recipientPast": ["a kneaded"]},</v>
@@ -15193,7 +15186,7 @@
         <v>1905</v>
       </c>
     </row>
-    <row r="92" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A92" t="str">
         <f t="shared" si="14"/>
         <v>{"spelling": "hoe", "group": "_o", "pos": "Noun", "adult": false, "has": ["a handle"], "in": ["a farm","a farmyard","a field"], "on": [], "from": ["a farm","a farmyard","a field"], "is": [], "typeOf": ["a tool","a farm tool"], "supertypeOf": [], "nearlyIs": ["a plough"], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -15290,7 +15283,7 @@
         <v>1134</v>
       </c>
     </row>
-    <row r="93" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A93" t="str">
         <f t="shared" si="14"/>
         <v>{"spelling": "ho", "group": "_o", "pos": "Noun", "adult": true, "has": ["a pimp","fishnets"], "in": ["a dark alley","a brothel"], "on": ["the streets","a street corner"], "from": ["a brothel"], "is": ["a prostitute","a slag","a hooker"], "typeOf": [], "supertypeOf": [], "nearlyIs": [], "property": ["a skanky","a slutty"], "acts": ["shags","fucks","sucks"], "actsCont": ["a shagging","a fucking"], "recipient": ["shag","fuck","sleep with"], "recipientPast": []},</v>
@@ -15420,7 +15413,7 @@
         <v>1911</v>
       </c>
     </row>
-    <row r="94" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A94" t="str">
         <f t="shared" si="14"/>
         <v>{"spelling": "beau", "group": "_o", "pos": "Noun", "adult": false, "has": ["a lover"], "in": [], "on": [], "from": [], "is": ["a lover"], "typeOf": [], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": ["loves"], "actsCont": ["a loving"], "recipient": ["love"], "recipientPast": ["a beloved"]},</v>
@@ -15505,7 +15498,7 @@
         <v>1915</v>
       </c>
     </row>
-    <row r="95" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A95" t="str">
         <f t="shared" si="14"/>
         <v>{"spelling": "no", "group": "_o", "pos": "Noun", "adult": false, "has": [], "in": [], "on": [], "from": [], "is": [], "typeOf": [], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": [], "actsCont": ["a missing","a lacking"], "recipient": [], "recipientPast": []},</v>
@@ -15648,7 +15641,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="97" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A97" t="str">
         <f t="shared" si="14"/>
         <v>{"spelling": "mo", "group": "_o", "pos": "Noun", "adult": false, "has": [], "in": ["a moment"], "on": [], "from": [], "is": ["a moment","a second"], "typeOf": ["a time period"], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -15727,7 +15720,7 @@
         <v>945</v>
       </c>
     </row>
-    <row r="98" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A98" t="str">
         <f t="shared" si="14"/>
         <v>{"spelling": "snow", "group": "_o", "pos": "Noun", "adult": false, "has": [], "in": ["winter"], "on": ["a mountain"], "from": [], "is": [], "typeOf": ["weather","precipitation"], "supertypeOf": [], "nearlyIs": ["ice"], "property": ["a cold","a chilly"], "acts": ["thaws","freezes"], "actsCont": [], "recipient": ["forecast"], "recipientPast": []},</v>
@@ -15824,7 +15817,7 @@
         <v>1920</v>
       </c>
     </row>
-    <row r="99" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A99" t="str">
         <f t="shared" si="14"/>
         <v>{"spelling": "throw", "group": "_o", "pos": "Noun", "adult": false, "has": [], "in": [], "on": [], "from": ["a pitcher","a bowler"], "is": [], "typeOf": ["an action"], "supertypeOf": ["a launch"], "nearlyIs": [], "property": [], "acts": ["hits","misses"], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -15909,7 +15902,7 @@
         <v>1922</v>
       </c>
     </row>
-    <row r="100" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A100" t="str">
         <f t="shared" si="14"/>
         <v>{"spelling": "show", "group": "_o", "pos": "Noun", "adult": false, "has": ["actors","an audience","a stage"], "in": [], "on": ["stage","tv","Broadway"], "from": [], "is": ["a presentation"], "typeOf": ["an event"], "supertypeOf": ["a play","an opera","a circus"], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": ["watch","perform"], "recipientPast": ["a watched","an acted","a performed"]},</v>
@@ -16024,7 +16017,7 @@
         <v>1893</v>
       </c>
     </row>
-    <row r="101" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A101" t="str">
         <f t="shared" si="14"/>
         <v>{"spelling": "foe", "group": "_o", "pos": "Noun", "adult": false, "has": ["a vendetta"], "in": [], "on": [], "from": [], "is": ["an enemy","an adversary","an opponent"], "typeOf": [], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": ["defeat"], "recipientPast": []},</v>
@@ -16106,7 +16099,7 @@
         <v>1926</v>
       </c>
     </row>
-    <row r="102" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A102" t="str">
         <f t="shared" si="14"/>
         <v>{"spelling": "rite", "group": "_ite", "pos": "Noun", "adult": false, "has": ["candles","cultists","a sacrifice"], "in": [], "on": ["an altar"], "from": [], "is": [], "typeOf": ["a ceremony"], "supertypeOf": ["a sacrifice","a blood sacrifice","a funeral"], "nearlyIs": ["a spell"], "property": ["a ceremonial","a religious"], "acts": [], "actsCont": [], "recipient": ["perform"], "recipientPast": ["a performed"]},</v>
@@ -16212,7 +16205,7 @@
         <v>1893</v>
       </c>
     </row>
-    <row r="103" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A103" t="str">
         <f t="shared" si="14"/>
         <v>{"spelling": "right", "group": "_ite", "pos": "Noun", "adult": false, "has": [], "in": [], "on": [], "from": [], "is": [], "typeOf": [], "supertypeOf": [], "nearlyIs": ["a permission"], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -16282,7 +16275,7 @@
         <v>1153</v>
       </c>
     </row>
-    <row r="104" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A104" t="str">
         <f t="shared" si="14"/>
         <v>{"spelling": "site", "group": "_ite", "pos": "Noun", "adult": false, "has": ["a location","a URL"], "in": [], "on": [], "from": [], "is": ["a plot"], "typeOf": ["an area"], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -16361,7 +16354,7 @@
         <v>1102</v>
       </c>
     </row>
-    <row r="105" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A105" t="str">
         <f t="shared" si="14"/>
         <v>{"spelling": "sight", "group": "_ite", "pos": "Noun", "adult": false, "has": ["eyes"], "in": [], "on": [], "from": [], "is": ["a view"], "typeOf": [], "supertypeOf": [], "nearlyIs": ["a scene"], "property": ["a beautiful"], "acts": [], "actsCont": [], "recipient": ["see","view","watch"], "recipientPast": ["a viewed","a watched"]},</v>
@@ -16455,7 +16448,7 @@
         <v>1924</v>
       </c>
     </row>
-    <row r="106" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A106" t="str">
         <f t="shared" si="14"/>
         <v>{"spelling": "fight", "group": "_ite", "pos": "Noun", "adult": false, "has": ["combatants","warriors","punches"], "in": [], "on": [], "from": [], "is": [], "typeOf": ["an argument","a disagreement"], "supertypeOf": ["a battle","a spat","combat"], "nearlyIs": [], "property": ["an aggressive"], "acts": [], "actsCont": [], "recipient": ["win","lose"], "recipientPast": []},</v>
@@ -16555,7 +16548,7 @@
         <v>1929</v>
       </c>
     </row>
-    <row r="107" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A107" t="str">
         <f t="shared" si="14"/>
         <v>{"spelling": "kite", "group": "_ite", "pos": "Noun", "adult": false, "has": ["a string"], "in": ["the sky"], "on": [], "from": [], "is": [], "typeOf": ["a toy","a bird"], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": ["flies"], "actsCont": ["a flying"], "recipient": [], "recipientPast": []},</v>
@@ -16640,7 +16633,7 @@
         <v>1701</v>
       </c>
     </row>
-    <row r="108" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A108" t="str">
         <f t="shared" si="14"/>
         <v>{"spelling": "light", "group": "_ite", "pos": "Noun", "adult": false, "has": ["a switch"], "in": [], "on": [], "from": ["the sun","a lamp","a torch"], "is": [], "typeOf": [], "supertypeOf": ["a lantern","a torch","a lamp"], "nearlyIs": [], "property": ["a bright"], "acts": ["shines","glows"], "actsCont": ["a shining","a glowing"], "recipient": ["put out"], "recipientPast": []},</v>
@@ -16746,7 +16739,7 @@
         <v>1932</v>
       </c>
     </row>
-    <row r="109" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A109" t="str">
         <f t="shared" si="14"/>
         <v>{"spelling": "bite", "group": "_ite", "pos": "Noun", "adult": false, "has": ["teeth","teethmarks"], "in": [], "on": [], "from": ["a wild animal","a dog"], "is": [], "typeOf": [], "supertypeOf": ["a chomp"], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -16898,7 +16891,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="111" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A111" t="str">
         <f t="shared" si="14"/>
         <v>{"spelling": "byte", "group": "_ite", "pos": "Noun", "adult": false, "has": ["data","memory"], "in": ["a computer"], "on": ["the computer"], "from": [], "is": [], "typeOf": ["memory"], "supertypeOf": [], "nearlyIs": [], "property": ["an electronic"], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -16983,7 +16976,7 @@
         <v>1703</v>
       </c>
     </row>
-    <row r="112" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A112" t="str">
         <f t="shared" si="14"/>
         <v>{"spelling": "night", "group": "_ite", "pos": "Noun", "adult": false, "has": ["a moon","stars"], "in": ["the evening"], "on": [], "from": [], "is": [], "typeOf": ["a time period"], "supertypeOf": ["an evening"], "nearlyIs": ["darkness","a sunset"], "property": ["a dark"], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -17074,7 +17067,7 @@
         <v>1704</v>
       </c>
     </row>
-    <row r="113" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A113" t="str">
         <f t="shared" si="14"/>
         <v>{"spelling": "knight", "group": "_ite", "pos": "Noun", "adult": false, "has": ["a horse","a sword","a shield"], "in": ["the middle ages","a joust"], "on": ["a chess-board","a horse"], "from": ["the middle ages"], "is": ["a sir"], "typeOf": ["a warrior"], "supertypeOf": ["a cavalier"], "nearlyIs": ["a gentleman"], "property": ["an honorable","a medieval","an armoured"], "acts": ["fights","rides"], "actsCont": ["a fighting","a riding"], "recipient": [], "recipientPast": []},</v>
@@ -17268,7 +17261,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="115" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A115" t="str">
         <f t="shared" si="14"/>
         <v>{"spelling": "mite", "group": "_ite", "pos": "Noun", "adult": false, "has": ["lots of legs"], "in": [], "on": [], "from": [], "is": [], "typeOf": ["an insect"], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -17341,7 +17334,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="116" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A116" t="str">
         <f t="shared" si="14"/>
         <v>{"spelling": "shite", "group": "_ite", "pos": "Noun", "adult": true, "has": ["a bad smell","a bit of sweetcorn in it"], "in": ["the toilet"], "on": [], "from": [], "is": ["a turd","a crap","faeces"], "typeOf": ["a dump","a floater","a bodily function"], "supertypeOf": ["diarrhea"], "nearlyIs": ["rubbish","junk"], "property": ["a smelly","a rubbish"], "acts": ["stinks","smells"], "actsCont": ["a stinking"], "recipient": ["flush"], "recipientPast": []},</v>
@@ -17465,7 +17458,7 @@
         <v>1846</v>
       </c>
     </row>
-    <row r="117" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A117" t="str">
         <f t="shared" si="14"/>
         <v>{"spelling": "two", "group": "_ew", "pos": "Noun", "adult": false, "has": [], "in": ["pairs"], "on": [], "from": [], "is": ["a pair","a duo","a couple"], "typeOf": ["a number"], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -17547,7 +17540,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="118" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A118" t="str">
         <f t="shared" si="14"/>
         <v>{"spelling": "yew", "group": "_ew", "pos": "Noun", "adult": false, "has": ["leaves","bark","branches"], "in": ["a forest","a wood","the woods"], "on": [], "from": [], "is": [], "typeOf": ["a tree","a plant"], "supertypeOf": [], "nearlyIs": [], "property": ["a leafy"], "acts": [], "actsCont": [], "recipient": ["chop down"], "recipientPast": []},</v>
@@ -17644,7 +17637,7 @@
         <v>1808</v>
       </c>
     </row>
-    <row r="119" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A119" t="str">
         <f t="shared" si="14"/>
         <v>{"spelling": "pew", "group": "_ew", "pos": "Noun", "adult": false, "has": ["bibles"], "in": ["a church","a chapel"], "on": [], "from": [], "is": [], "typeOf": ["a seat","a bench","furniture"], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": ["sit on"], "recipientPast": []},</v>
@@ -17732,7 +17725,7 @@
         <v>1937</v>
       </c>
     </row>
-    <row r="120" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A120" t="str">
         <f t="shared" si="14"/>
         <v>{"spelling": "dew", "group": "_ew", "pos": "Noun", "adult": false, "has": [], "in": [], "on": ["the grass","the morning"], "from": [], "is": [], "typeOf": ["water","precipitation"], "supertypeOf": [], "nearlyIs": ["a mist"], "property": ["a damp"], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -17817,7 +17810,7 @@
         <v>1708</v>
       </c>
     </row>
-    <row r="121" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A121" t="str">
         <f t="shared" si="14"/>
         <v>{"spelling": "few", "group": "_ew", "pos": "Noun", "adult": false, "has": [], "in": [], "on": [], "from": [], "is": ["a handful"], "typeOf": ["an amount","a number"], "supertypeOf": [], "nearlyIs": ["a couple"], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -17896,7 +17889,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="122" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A122" t="str">
         <f t="shared" ref="A122:A185" si="28">CONCATENATE("{""spelling"": """,Q122,""", ""group"": """,O122,""", ""pos"": """,S122,""", ""adult"": ",IF(R122=TRUE,"true","false"),", ""has"": [",B122,"]",", ""in"": [",C122,"]",", ""on"": [",D122,"]",", ""from"": [",E122,"]",", ""is"": [",F122,"]",", ""typeOf"": [",G122,"]",", ""supertypeOf"": [",H122,"]",", ""nearlyIs"": [",I122,"]",", ""property"": [",J122,"]",", ""acts"": [",K122,"]",", ""actsCont"": [",L122,"]",", ""recipient"": [",M122,"]",", ""recipientPast"": [",N122,"]},")</f>
         <v>{"spelling": "hue", "group": "_ew", "pos": "Noun", "adult": false, "has": [], "in": ["a colour palette"], "on": [], "from": [], "is": [], "typeOf": ["a colour","a shade"], "supertypeOf": [], "nearlyIs": [], "property": ["a colourful"], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -17975,7 +17968,7 @@
         <v>1709</v>
       </c>
     </row>
-    <row r="123" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A123" t="str">
         <f t="shared" si="28"/>
         <v>{"spelling": "jew", "group": "_ew", "pos": "Noun", "adult": true, "has": ["a circumcision"], "in": ["a synagogue"], "on": [], "from": ["Israel"], "is": ["a jewish person"], "typeOf": ["a believer"], "supertypeOf": ["a Rabbi"], "nearlyIs": [], "property": ["a religious"], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -18066,7 +18059,7 @@
         <v>1697</v>
       </c>
     </row>
-    <row r="124" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A124" t="str">
         <f t="shared" si="28"/>
         <v>{"spelling": "loo", "group": "_ew", "pos": "Noun", "adult": false, "has": ["a flush"], "in": ["a bathroom","a restroom"], "on": [], "from": [], "is": ["a toilet","a bathroom"], "typeOf": [], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": ["pee in","poop on","flush"], "recipientPast": ["a flushed"]},</v>
@@ -18160,7 +18153,7 @@
         <v>1892</v>
       </c>
     </row>
-    <row r="125" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A125" t="str">
         <f t="shared" si="28"/>
         <v>{"spelling": "zoo", "group": "_ew", "pos": "Noun", "adult": false, "has": ["animals","lions","tigers"], "in": [], "on": [], "from": [], "is": [], "typeOf": [], "supertypeOf": [], "nearlyIs": ["a stable"], "property": [], "acts": [], "actsCont": [], "recipient": ["visit"], "recipientPast": ["a visited"]},</v>
@@ -18245,7 +18238,7 @@
         <v>1941</v>
       </c>
     </row>
-    <row r="126" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A126" t="str">
         <f t="shared" si="28"/>
         <v>{"spelling": "view", "group": "_ew", "pos": "Noun", "adult": false, "has": [], "in": [], "on": ["a mountain top"], "from": ["an overlook","a beauty spot","a skyscraper"], "is": ["a sight"], "typeOf": [], "supertypeOf": [], "nearlyIs": ["a scene"], "property": ["a beautiful"], "acts": [], "actsCont": [], "recipient": ["see","look at"], "recipientPast": ["a seen"]},</v>
@@ -18342,7 +18335,7 @@
         <v>1943</v>
       </c>
     </row>
-    <row r="127" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A127" t="str">
         <f t="shared" si="28"/>
         <v>{"spelling": "boo", "group": "_ew", "pos": "Noun", "adult": false, "has": [], "in": [], "on": [], "from": ["a ghost"], "is": [], "typeOf": ["a fright","a scare"], "supertypeOf": [], "nearlyIs": ["a scream","a shout"], "property": ["a frightful","a scary"], "acts": ["scares people"], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -18433,7 +18426,7 @@
         <v>1944</v>
       </c>
     </row>
-    <row r="128" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A128" t="str">
         <f t="shared" si="28"/>
         <v>{"spelling": "spew", "group": "_ew", "pos": "Noun", "adult": true, "has": ["a bit of sweetcorn in it","a bad smell"], "in": [], "on": ["the pavement"], "from": ["a drunk"], "is": ["vomit"], "typeOf": [], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": ["clean up"], "recipientPast": []},</v>
@@ -18521,7 +18514,7 @@
         <v>1945</v>
       </c>
     </row>
-    <row r="129" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A129" t="str">
         <f t="shared" si="28"/>
         <v>{"spelling": "shoe", "group": "_ew", "pos": "Noun", "adult": false, "has": ["laces","a sole"], "in": [], "on": ["your foot","a foot"], "from": [], "is": [], "typeOf": ["footwear"], "supertypeOf": ["a sandal","a high heel","a slipper"], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": ["wear"], "recipientPast": ["a worn"]},</v>
@@ -18618,7 +18611,7 @@
         <v>1886</v>
       </c>
     </row>
-    <row r="130" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A130" t="str">
         <f t="shared" si="28"/>
         <v>{"spelling": "stew", "group": "_ew", "pos": "Noun", "adult": false, "has": ["meat in it","carrots"], "in": [], "on": [], "from": ["a kitchen","the kitchen"], "is": [], "typeOf": ["a meal","a main course"], "supertypeOf": [], "nearlyIs": [], "property": ["a meaty"], "acts": ["simmers","boils"], "actsCont": ["a simmering","a boiling"], "recipient": ["eat","cook"], "recipientPast": ["a cooked"]},</v>
@@ -18727,7 +18720,7 @@
         <v>1894</v>
       </c>
     </row>
-    <row r="131" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A131" t="str">
         <f t="shared" si="28"/>
         <v>{"spelling": "you", "group": "_ew", "pos": "Noun", "adult": false, "has": ["no friends","a bad attitude","a bad smell"], "in": ["terrible shape"], "on": [], "from": [], "is": ["an idiot","a moron","a jerk"], "typeOf": [], "supertypeOf": [], "nearlyIs": [], "property": ["a terrible","an awful","an ugly"], "acts": ["smells","stinks"], "actsCont": ["a stinking"], "recipient": [], "recipientPast": []},</v>
@@ -18833,7 +18826,7 @@
         <v>1878</v>
       </c>
     </row>
-    <row r="132" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A132" t="str">
         <f t="shared" si="28"/>
         <v>{"spelling": "ring", "group": "_ing", "pos": "Noun", "adult": false, "has": ["an inscription"], "in": [], "on": ["your finger","a finger"], "from": ["a jewellers"], "is": [], "typeOf": ["jewellery"], "supertypeOf": [], "nearlyIs": ["a circle"], "property": [], "acts": [], "actsCont": [], "recipient": ["wear"], "recipientPast": ["a worn"]},</v>
@@ -18924,7 +18917,7 @@
         <v>1886</v>
       </c>
     </row>
-    <row r="133" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A133" t="str">
         <f t="shared" si="28"/>
         <v>{"spelling": "wing", "group": "_ing", "pos": "Noun", "adult": false, "has": ["feathers"], "in": [], "on": [], "from": [], "is": [], "typeOf": [], "supertypeOf": [], "nearlyIs": ["a side"], "property": ["a feathered"], "acts": ["flaps"], "actsCont": ["a flapping"], "recipient": [], "recipientPast": []},</v>
@@ -19006,7 +18999,7 @@
         <v>1951</v>
       </c>
     </row>
-    <row r="134" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A134" t="str">
         <f t="shared" si="28"/>
         <v>{"spelling": "thing", "group": "_ing", "pos": "Noun", "adult": false, "has": [], "in": [], "on": [], "from": [], "is": ["an item","an object"], "typeOf": [], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -19079,7 +19072,7 @@
         <v>982</v>
       </c>
     </row>
-    <row r="135" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A135" t="str">
         <f t="shared" si="28"/>
         <v>{"spelling": "ying", "group": "_ing", "pos": "Noun", "adult": false, "has": ["a yang"], "in": [], "on": [], "from": [], "is": [], "typeOf": [], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -19149,7 +19142,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="136" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A136" t="str">
         <f t="shared" si="28"/>
         <v>{"spelling": "ping", "group": "_ing", "pos": "Noun", "adult": false, "has": ["lag"], "in": [], "on": ["a network"], "from": [], "is": [], "typeOf": ["a noise","a sound","an alert"], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": ["hear"], "recipientPast": []},</v>
@@ -19234,7 +19227,7 @@
         <v>1959</v>
       </c>
     </row>
-    <row r="137" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A137" t="str">
         <f t="shared" si="28"/>
         <v>{"spelling": "ding", "group": "_ing", "pos": "Noun", "adult": false, "has": [], "in": [], "on": [], "from": [], "is": [], "typeOf": ["a noise","a sound","an alert"], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": ["hear"], "recipientPast": []},</v>
@@ -19313,7 +19306,7 @@
         <v>1959</v>
       </c>
     </row>
-    <row r="138" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A138" t="str">
         <f t="shared" si="28"/>
         <v>{"spelling": "king", "group": "_ing", "pos": "Noun", "adult": false, "has": ["subjects","a country","a crown"], "in": ["the throne room","the palace"], "on": ["a throne"], "from": ["the palace"], "is": ["a monarch"], "typeOf": ["a ruler"], "supertypeOf": [], "nearlyIs": ["an emperor","a prince"], "property": ["a royal"], "acts": ["rules","reigns"], "actsCont": ["a ruling","a reigning"], "recipient": [], "recipientPast": []},</v>
@@ -19428,7 +19421,7 @@
         <v>1954</v>
       </c>
     </row>
-    <row r="139" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A139" t="str">
         <f t="shared" si="28"/>
         <v>{"spelling": "app", "group": "_ap", "pos": "Noun", "adult": false, "has": ["developers","a developer"], "in": [], "on": ["your phone","a phone"], "from": [], "is": ["an application"], "typeOf": ["a program"], "supertypeOf": ["a mobile game","WhatsApp"], "nearlyIs": ["a game"], "property": ["a digital"], "acts": [], "actsCont": [], "recipient": ["install","uninstall"], "recipientPast": ["an installed"]},</v>
@@ -19534,7 +19527,7 @@
         <v>1956</v>
       </c>
     </row>
-    <row r="140" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A140" t="str">
         <f t="shared" si="28"/>
         <v>{"spelling": "rap", "group": "_ap", "pos": "Noun", "adult": false, "has": ["lyrics"], "in": [], "on": ["the radio","Spotify"], "from": [], "is": [], "typeOf": ["music","singing"], "supertypeOf": [], "nearlyIs": ["a song"], "property": ["a musical"], "acts": [], "actsCont": [], "recipient": ["listen to","hear"], "recipientPast": []},</v>
@@ -19628,7 +19621,7 @@
         <v>1959</v>
       </c>
     </row>
-    <row r="141" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A141" t="str">
         <f t="shared" si="28"/>
         <v>{"spelling": "tap", "group": "_ap", "pos": "Noun", "adult": false, "has": [], "in": ["the kitchen"], "on": [], "from": [], "is": [], "typeOf": ["a touch"], "supertypeOf": [], "nearlyIs": ["a prod"], "property": [], "acts": ["drips"], "actsCont": ["a dripping"], "recipient": [], "recipientPast": []},</v>
@@ -19710,7 +19703,7 @@
         <v>1961</v>
       </c>
     </row>
-    <row r="142" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A142" t="str">
         <f t="shared" si="28"/>
         <v>{"spelling": "yap", "group": "_ap", "pos": "Noun", "adult": false, "has": [], "in": [], "on": [], "from": ["a small dog","a puppy","a dog"], "is": [], "typeOf": ["a bark"], "supertypeOf": [], "nearlyIs": ["a squeal"], "property": [], "acts": [], "actsCont": [], "recipient": ["hear"], "recipientPast": []},</v>
@@ -19795,7 +19788,7 @@
         <v>1959</v>
       </c>
     </row>
-    <row r="143" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A143" t="str">
         <f t="shared" si="28"/>
         <v>{"spelling": "sap", "group": "_ap", "pos": "Noun", "adult": false, "has": [], "in": [], "on": ["a tree"], "from": ["a tree"], "is": [], "typeOf": [], "supertypeOf": ["maple syrup"], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -19871,7 +19864,7 @@
         <v>1222</v>
       </c>
     </row>
-    <row r="144" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A144" t="str">
         <f t="shared" si="28"/>
         <v>{"spelling": "gap", "group": "_ap", "pos": "Noun", "adult": false, "has": [], "in": [], "on": [], "from": [], "is": ["an opening"], "typeOf": ["a space"], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -19944,7 +19937,7 @@
         <v>1223</v>
       </c>
     </row>
-    <row r="145" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A145" t="str">
         <f t="shared" si="28"/>
         <v>{"spelling": "lap", "group": "_ap", "pos": "Noun", "adult": false, "has": [], "in": [], "on": [], "from": [], "is": [], "typeOf": [], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -20011,7 +20004,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="146" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A146" t="str">
         <f t="shared" si="28"/>
         <v>{"spelling": "clap", "group": "_ap", "pos": "Noun", "adult": false, "has": ["a noise","two hands"], "in": [], "on": [], "from": ["the audience","an audience"], "is": [], "typeOf": ["a sound"], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": ["hear"], "recipientPast": []},</v>
@@ -20096,7 +20089,7 @@
         <v>1959</v>
       </c>
     </row>
-    <row r="147" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A147" t="str">
         <f t="shared" si="28"/>
         <v>{"spelling": "cap", "group": "_ap", "pos": "Noun", "adult": false, "has": ["a brim"], "in": [], "on": ["your head","a bottle"], "from": [], "is": [], "typeOf": ["a hat","a lid"], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": ["wear"], "recipientPast": ["a worn"]},</v>
@@ -20184,7 +20177,7 @@
         <v>1886</v>
       </c>
     </row>
-    <row r="148" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A148" t="str">
         <f t="shared" si="28"/>
         <v>{"spelling": "bap", "group": "_ap", "pos": "Noun", "adult": false, "has": ["a filling","bread"], "in": [], "on": [], "from": ["a baker"], "is": [], "typeOf": ["a bun","a bread","a baked good"], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": ["bake"], "recipientPast": ["a baked"]},</v>
@@ -20275,7 +20268,7 @@
         <v>1902</v>
       </c>
     </row>
-    <row r="149" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A149" t="str">
         <f t="shared" si="28"/>
         <v>{"spelling": "nap", "group": "_ap", "pos": "Noun", "adult": false, "has": ["a pillow"], "in": ["bed"], "on": ["the sofa"], "from": [], "is": [], "typeOf": ["a sleep","a rest"], "supertypeOf": [], "nearlyIs": [], "property": ["a sleepy"], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -20360,7 +20353,7 @@
         <v>1720</v>
       </c>
     </row>
-    <row r="150" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A150" t="str">
         <f t="shared" si="28"/>
         <v>{"spelling": "map", "group": "_ap", "pos": "Noun", "adult": false, "has": ["a landscape","oceans","continents"], "in": ["an atlas"], "on": [], "from": [], "is": [], "typeOf": [], "supertypeOf": ["an atlas","a globe"], "nearlyIs": ["a plan"], "property": [], "acts": [], "actsCont": [], "recipient": ["draw","navigate with"], "recipientPast": []},</v>
@@ -20454,7 +20447,7 @@
         <v>1962</v>
       </c>
     </row>
-    <row r="151" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A151" t="str">
         <f t="shared" si="28"/>
         <v>{"spelling": "trap", "group": "_ap", "pos": "Noun", "adult": false, "has": ["bait"], "in": [], "on": [], "from": ["a hunter"], "is": [], "typeOf": [], "supertypeOf": ["a snare","a pit","a pitfall"], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -20536,7 +20529,7 @@
         <v>1233</v>
       </c>
     </row>
-    <row r="152" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A152" t="str">
         <f t="shared" si="28"/>
         <v>{"spelling": "chap", "group": "_ap", "pos": "Noun", "adult": false, "has": ["tophat","monocle"], "in": ["England"], "on": [], "from": ["England"], "is": ["a gent"], "typeOf": ["a person"], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -20621,7 +20614,7 @@
         <v>994</v>
       </c>
     </row>
-    <row r="153" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A153" t="str">
         <f t="shared" si="28"/>
         <v>{"spelling": "snap", "group": "_ap", "pos": "Noun", "adult": false, "has": [], "in": [], "on": [], "from": [], "is": ["a picture"], "typeOf": [], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": ["hear"], "recipientPast": []},</v>
@@ -20694,7 +20687,7 @@
         <v>1959</v>
       </c>
     </row>
-    <row r="154" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A154" t="str">
         <f t="shared" si="28"/>
         <v>{"spelling": "jam", "group": "_am", "pos": "Noun", "adult": false, "has": ["fruit","sugar","strawberries"], "in": ["the kitchen","a jar"], "on": ["toast"], "from": [], "is": ["a preserve"], "typeOf": ["a spread"], "supertypeOf": [], "nearlyIs": ["a jelly"], "property": ["a fruity","a sweet"], "acts": [], "actsCont": [], "recipient": ["eat","spread"], "recipientPast": ["a spread"]},</v>
@@ -20803,7 +20796,7 @@
         <v>1238</v>
       </c>
     </row>
-    <row r="155" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A155" t="str">
         <f t="shared" si="28"/>
         <v>{"spelling": "ram", "group": "_am", "pos": "Noun", "adult": false, "has": ["horns","wool","hooves"], "in": ["a field"], "on": [], "from": ["a field","a farm"], "is": [], "typeOf": ["a sheep","a farm animal","an animal"], "supertypeOf": [], "nearlyIs": [], "property": ["a wooly","a horned"], "acts": ["bleats"], "actsCont": ["a bleating"], "recipient": ["shear"], "recipientPast": ["a sheared"]},</v>
@@ -20915,7 +20908,7 @@
         <v>1965</v>
       </c>
     </row>
-    <row r="156" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A156" t="str">
         <f t="shared" si="28"/>
         <v>{"spelling": "tram", "group": "_am", "pos": "Noun", "adult": false, "has": ["passengers","rails"], "in": [], "on": ["rails"], "from": [], "is": [], "typeOf": ["a vehicle"], "supertypeOf": ["a streetcar"], "nearlyIs": ["a train","a carriage"], "property": [], "acts": ["drives"], "actsCont": ["a driving"], "recipient": ["board","ride"], "recipientPast": []},</v>
@@ -21015,7 +21008,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="157" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A157" t="str">
         <f t="shared" si="28"/>
         <v>{"spelling": "spam", "group": "_am", "pos": "Noun", "adult": false, "has": [], "in": ["your inbox"], "on": [], "from": ["a scammer"], "is": ["junkmail"], "typeOf": [], "supertypeOf": [], "nearlyIs": ["an email"], "property": ["a canned","a repetetive"], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -21100,7 +21093,7 @@
         <v>1725</v>
       </c>
     </row>
-    <row r="158" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A158" t="str">
         <f t="shared" si="28"/>
         <v>{"spelling": "slam", "group": "_am", "pos": "Noun", "adult": false, "has": [], "in": [], "on": [], "from": [], "is": ["a smash"], "typeOf": [], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -21170,7 +21163,7 @@
         <v>1244</v>
       </c>
     </row>
-    <row r="159" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A159" t="str">
         <f t="shared" si="28"/>
         <v>{"spelling": "scam", "group": "_am", "pos": "Noun", "adult": false, "has": ["a victim"], "in": [], "on": [], "from": ["a spammer","a conman"], "is": ["a con"], "typeOf": ["a lie","a ploy"], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": ["fall for"], "recipientPast": []},</v>
@@ -21258,7 +21251,7 @@
         <v>1969</v>
       </c>
     </row>
-    <row r="160" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A160" t="str">
         <f t="shared" si="28"/>
         <v>{"spelling": "dam", "group": "_am", "pos": "Noun", "adult": false, "has": ["a lot of water"], "in": ["the river","a river"], "on": [], "from": [], "is": [], "typeOf": ["a blockade"], "supertypeOf": [], "nearlyIs": [], "property": ["a blocked"], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -21407,7 +21400,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="162" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A162" t="str">
         <f t="shared" si="28"/>
         <v>{"spelling": "damn", "group": "_am", "pos": "Noun", "adult": true, "has": [], "in": [], "on": [], "from": ["a sinner"], "is": [], "typeOf": ["swearing","a curse"], "supertypeOf": [], "nearlyIs": [], "property": ["a cursed"], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -21489,7 +21482,7 @@
         <v>1727</v>
       </c>
     </row>
-    <row r="163" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A163" t="str">
         <f t="shared" si="28"/>
         <v>{"spelling": "ham", "group": "_am", "pos": "Noun", "adult": false, "has": ["bone"], "in": ["a sandwich"], "on": [], "from": ["a pig"], "is": [], "typeOf": ["pork","meat"], "supertypeOf": [], "nearlyIs": [], "property": ["a meaty"], "acts": [], "actsCont": [], "recipient": ["eat"], "recipientPast": []},</v>
@@ -21577,7 +21570,7 @@
         <v>1861</v>
       </c>
     </row>
-    <row r="164" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A164" t="str">
         <f t="shared" si="28"/>
         <v>{"spelling": "lamb", "group": "_am", "pos": "Noun", "adult": false, "has": ["wool","hooves"], "in": ["a field"], "on": [], "from": ["a field","a farm"], "is": [], "typeOf": ["sheep","meat","a farm animal"], "supertypeOf": [], "nearlyIs": [], "property": ["a wooly"], "acts": ["bleats"], "actsCont": ["a bleating"], "recipient": ["shear","eat"], "recipientPast": ["a sheared"]},</v>
@@ -21686,7 +21679,7 @@
         <v>1965</v>
       </c>
     </row>
-    <row r="165" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A165" t="str">
         <f t="shared" si="28"/>
         <v>{"spelling": "clam", "group": "_am", "pos": "Noun", "adult": false, "has": ["a shell","a pearl"], "in": ["the ocean","the sea"], "on": [], "from": ["a fishmonger"], "is": [], "typeOf": ["a shellfish","a sea creature","a crustacean"], "supertypeOf": [], "nearlyIs": ["an oyster"], "property": [], "acts": [], "actsCont": [], "recipient": ["shell"], "recipientPast": []},</v>
@@ -21783,7 +21776,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="166" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A166" t="str">
         <f t="shared" si="28"/>
         <v>{"spelling": "day", "group": "_ay", "pos": "Noun", "adult": false, "has": ["a morning","an afternoon","the sun"], "in": ["the morning","the afternoon"], "on": [], "from": [], "is": [], "typeOf": ["a time period"], "supertypeOf": [], "nearlyIs": ["a morning","an afternoon"], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -21874,7 +21867,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="167" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A167" t="str">
         <f t="shared" si="28"/>
         <v>{"spelling": "way", "group": "_ay", "pos": "Noun", "adult": false, "has": ["a signpost"], "in": [], "on": [], "from": [], "is": ["a path","a route","a trail"], "typeOf": [], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -21953,7 +21946,7 @@
         <v>1259</v>
       </c>
     </row>
-    <row r="168" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A168" t="str">
         <f t="shared" si="28"/>
         <v>{"spelling": "ray", "group": "_ay", "pos": "Noun", "adult": false, "has": ["gills"], "in": ["the sea","the ocean"], "on": [], "from": ["the sun","a fishmonger"], "is": [], "typeOf": ["a fish","a beam"], "supertypeOf": ["a sunbeam","a manta"], "nearlyIs": [], "property": [], "acts": ["shines"], "actsCont": ["a shining"], "recipient": [], "recipientPast": []},</v>
@@ -22053,7 +22046,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="169" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A169" t="str">
         <f t="shared" si="28"/>
         <v>{"spelling": "fey", "group": "_ay", "pos": "Noun", "adult": false, "has": ["magical powers"], "in": [], "on": [], "from": [], "is": [], "typeOf": ["a mythical creature","a legend","a myth"], "supertypeOf": ["an elf","a pixie","a sprite"], "nearlyIs": [], "property": ["a magical","an elfin","a mythical"], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -22150,7 +22143,7 @@
         <v>1730</v>
       </c>
     </row>
-    <row r="170" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A170" t="str">
         <f t="shared" si="28"/>
         <v>{"spelling": "gay", "group": "_ay", "pos": "Noun", "adult": true, "has": ["a husband"], "in": ["a pride parade"], "on": ["grinder"], "from": [], "is": ["a homosexual"], "typeOf": ["a sexual preference"], "supertypeOf": ["a lesbian"], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -22238,7 +22231,7 @@
         <v>1270</v>
       </c>
     </row>
-    <row r="171" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A171" t="str">
         <f t="shared" si="28"/>
         <v>{"spelling": "hay", "group": "_ay", "pos": "Noun", "adult": false, "has": [], "in": ["a field","a bale"], "on": [], "from": [], "is": [], "typeOf": ["fodder"], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -22314,7 +22307,7 @@
         <v>1272</v>
       </c>
     </row>
-    <row r="172" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A172" t="str">
         <f t="shared" si="28"/>
         <v>{"spelling": "hey", "group": "_ay", "pos": "Noun", "adult": false, "has": [], "in": [], "on": [], "from": [], "is": ["a hello","a hi"], "typeOf": ["a salutation"], "supertypeOf": [], "nearlyIs": ["a wave"], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -22393,7 +22386,7 @@
         <v>1276</v>
       </c>
     </row>
-    <row r="173" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A173" t="str">
         <f t="shared" si="28"/>
         <v>{"spelling": "lay", "group": "_ay", "pos": "Noun", "adult": true, "has": ["foreplay","a climax","an orgasm"], "in": [], "on": ["tinder"], "from": ["tinder"], "is": ["a shag","a sexual partner","a lay"], "typeOf": [], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": ["shag","fuck"], "recipientPast": ["a shagged","a fucked"]},</v>
@@ -22499,7 +22492,7 @@
         <v>1888</v>
       </c>
     </row>
-    <row r="174" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A174" t="str">
         <f t="shared" si="28"/>
         <v>{"spelling": "bay", "group": "_ay", "pos": "Noun", "adult": false, "has": ["ships","a pier","a beach"], "in": ["a cove"], "on": [], "from": [], "is": ["a cove"], "typeOf": ["a coastline"], "supertypeOf": [], "nearlyIs": ["a port"], "property": [], "acts": [], "actsCont": [], "recipient": ["sail into","swim in"], "recipientPast": []},</v>
@@ -22593,7 +22586,7 @@
         <v>1972</v>
       </c>
     </row>
-    <row r="175" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A175" t="str">
         <f t="shared" si="28"/>
         <v>{"spelling": "tray", "group": "_ay", "pos": "Noun", "adult": false, "has": ["a rim"], "in": ["front of the tv"], "on": [], "from": [], "is": [], "typeOf": [], "supertypeOf": [], "nearlyIs": ["a plate"], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -22669,7 +22662,7 @@
         <v>1282</v>
       </c>
     </row>
-    <row r="176" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A176" t="str">
         <f t="shared" si="28"/>
         <v>{"spelling": "stay", "group": "_ay", "pos": "Noun", "adult": false, "has": [], "in": ["a hotel","a hostel","a resort"], "on": ["holiday","vacation"], "from": [], "is": [], "typeOf": ["a holiday","a vacation"], "supertypeOf": ["a hotel","a hostel","a resort"], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -22766,7 +22759,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="177" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A177" t="str">
         <f t="shared" si="28"/>
         <v>{"spelling": "bot", "group": "_ot", "pos": "Noun", "adult": false, "has": ["AI"], "in": [], "on": [], "from": [], "is": ["an AI","an artificial intelligence"], "typeOf": [], "supertypeOf": [], "nearlyIs": [], "property": ["a digital","a robotic"], "acts": [], "actsCont": [], "recipient": ["program"], "recipientPast": ["a programmed"]},</v>
@@ -22854,7 +22847,7 @@
         <v>2078</v>
       </c>
     </row>
-    <row r="178" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A178" t="str">
         <f t="shared" si="28"/>
         <v>{"spelling": "knot", "group": "_ot", "pos": "Noun", "adult": false, "has": [], "in": ["a piece of rope","a tie","a string"], "on": [], "from": ["a boyscout"], "is": [], "typeOf": ["a tie","a fastening"], "supertypeOf": [], "nearlyIs": [], "property": ["a tied"], "acts": [], "actsCont": [], "recipient": ["tie","untie"], "recipientPast": ["a tied"]},</v>
@@ -22951,7 +22944,7 @@
         <v>1777</v>
       </c>
     </row>
-    <row r="179" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A179" t="str">
         <f t="shared" si="28"/>
         <v>{"spelling": "clot", "group": "_ot", "pos": "Noun", "adult": false, "has": [], "in": [], "on": [], "from": [], "is": [], "typeOf": [], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -23018,7 +23011,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="180" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A180" t="str">
         <f t="shared" si="28"/>
         <v>{"spelling": "Scot", "group": "_ot", "pos": "Noun", "adult": false, "has": ["bagpipes","a tartan","a kilt"], "in": ["Scotland","Edinburgh","Glasgow"], "on": [], "from": ["Scotland"], "is": [], "typeOf": ["a Brit","a European"], "supertypeOf": [], "nearlyIs": [], "property": ["a Gaelic"], "acts": ["drinks whisky","plays the bagpipes"], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -23121,7 +23114,7 @@
         <v>2081</v>
       </c>
     </row>
-    <row r="181" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A181" t="str">
         <f t="shared" si="28"/>
         <v>{"spelling": "oat", "group": "_ote", "pos": "Noun", "adult": false, "has": [], "in": ["your porridge","a flapjack","granola"], "on": [], "from": [], "is": [], "typeOf": ["a grain","a cereal"], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": ["cook"], "recipientPast": ["a cooked"]},</v>
@@ -23209,7 +23202,7 @@
         <v>1894</v>
       </c>
     </row>
-    <row r="182" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A182" t="str">
         <f t="shared" si="28"/>
         <v>{"spelling": "boat", "group": "_ote", "pos": "Noun", "adult": false, "has": ["a mast","sails","a captain"], "in": ["port","a lake"], "on": ["the high seas","a lake"], "from": ["a shipwright"], "is": ["a ship"], "typeOf": ["a vehicle"], "supertypeOf": ["a yacht","a dinghy","a canoe"], "nearlyIs": [], "property": [], "acts": ["sails","floats"], "actsCont": ["a sailing","a floating"], "recipient": [], "recipientPast": []},</v>
@@ -23327,7 +23320,7 @@
         <v>1880</v>
       </c>
     </row>
-    <row r="183" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A183" t="str">
         <f t="shared" si="28"/>
         <v>{"spelling": "coat", "group": "_ote", "pos": "Noun", "adult": false, "has": ["a zip","a hood"], "in": [], "on": [], "from": [], "is": ["a jacket"], "typeOf": ["a garment","clothing"], "supertypeOf": ["an anorak"], "nearlyIs": ["a fleece"], "property": [], "acts": [], "actsCont": [], "recipient": ["wear"], "recipientPast": ["a worn"]},</v>
@@ -23421,7 +23414,7 @@
         <v>1886</v>
       </c>
     </row>
-    <row r="184" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A184" t="str">
         <f t="shared" si="28"/>
         <v>{"spelling": "sky", "group": "_ie", "pos": "Noun", "adult": false, "has": ["clouds","birds","an atmosphere"], "in": [], "on": [], "from": [], "is": [], "typeOf": [], "supertypeOf": [], "nearlyIs": ["space","the atmosphere"], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -23503,7 +23496,7 @@
         <v>1292</v>
       </c>
     </row>
-    <row r="185" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A185" t="str">
         <f t="shared" si="28"/>
         <v>{"spelling": "rye", "group": "_ie", "pos": "Noun", "adult": false, "has": [], "in": [], "on": [], "from": [], "is": [], "typeOf": ["a grain","a cereal","a flour"], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -23579,7 +23572,7 @@
         <v>1293</v>
       </c>
     </row>
-    <row r="186" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A186" t="str">
         <f t="shared" ref="A186:A249" si="42">CONCATENATE("{""spelling"": """,Q186,""", ""group"": """,O186,""", ""pos"": """,S186,""", ""adult"": ",IF(R186=TRUE,"true","false"),", ""has"": [",B186,"]",", ""in"": [",C186,"]",", ""on"": [",D186,"]",", ""from"": [",E186,"]",", ""is"": [",F186,"]",", ""typeOf"": [",G186,"]",", ""supertypeOf"": [",H186,"]",", ""nearlyIs"": [",I186,"]",", ""property"": [",J186,"]",", ""acts"": [",K186,"]",", ""actsCont"": [",L186,"]",", ""recipient"": [",M186,"]",", ""recipientPast"": [",N186,"]},")</f>
         <v>{"spelling": "tie", "group": "_ie", "pos": "Noun", "adult": false, "has": ["a pattern","a knot"], "in": [], "on": [], "from": [], "is": [], "typeOf": ["clothing","a garment","formal wear"], "supertypeOf": ["a cravat"], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": ["wear"], "recipientPast": ["a worn"]},</v>
@@ -23670,7 +23663,7 @@
         <v>1886</v>
       </c>
     </row>
-    <row r="187" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A187" t="str">
         <f t="shared" si="42"/>
         <v>{"spelling": "try", "group": "_ie", "pos": "Noun", "adult": false, "has": [], "in": [], "on": [], "from": [], "is": ["an attempt"], "typeOf": [], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": ["attempt"], "recipientPast": ["an attempted"]},</v>
@@ -23746,7 +23739,7 @@
         <v>1978</v>
       </c>
     </row>
-    <row r="188" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A188" t="str">
         <f t="shared" si="42"/>
         <v>{"spelling": "pie", "group": "_ie", "pos": "Noun", "adult": false, "has": ["a crust","a filling","a baker"], "in": [], "on": [], "from": ["a baker"], "is": [], "typeOf": ["a pastry"], "supertypeOf": [], "nearlyIs": ["a pasty","a tart","a pizza"], "property": ["a delicious"], "acts": [], "actsCont": [], "recipient": ["eat","bake"], "recipientPast": ["a baked"]},</v>
@@ -23849,7 +23842,7 @@
         <v>1902</v>
       </c>
     </row>
-    <row r="189" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A189" t="str">
         <f t="shared" si="42"/>
         <v>{"spelling": "pi", "group": "_ie", "pos": "Noun", "adult": false, "has": ["a lot of numbers"], "in": ["a textbook","an equation"], "on": ["a calculator"], "from": [], "is": [], "typeOf": ["a number"], "supertypeOf": [], "nearlyIs": [], "property": ["a mathematical"], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -23934,7 +23927,7 @@
         <v>1734</v>
       </c>
     </row>
-    <row r="190" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A190" t="str">
         <f t="shared" si="42"/>
         <v>{"spelling": "sigh", "group": "_ie", "pos": "Noun", "adult": false, "has": [], "in": [], "on": [], "from": [], "is": [], "typeOf": ["a noise","a sound"], "supertypeOf": [], "nearlyIs": ["a gasp","a whisper"], "property": [], "acts": [], "actsCont": [], "recipient": ["hear"], "recipientPast": []},</v>
@@ -24016,7 +24009,7 @@
         <v>1959</v>
       </c>
     </row>
-    <row r="191" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A191" t="str">
         <f t="shared" si="42"/>
         <v>{"spelling": "sty", "group": "_ie", "pos": "Noun", "adult": false, "has": ["a pig","muck","a trough"], "in": ["a farm"], "on": ["your eye","your eyelid"], "from": [], "is": [], "typeOf": ["a mark","a blemish"], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -24107,7 +24100,7 @@
         <v>1033</v>
       </c>
     </row>
-    <row r="192" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A192" t="str">
         <f t="shared" si="42"/>
         <v>{"spelling": "STI", "group": "_ie", "pos": "Noun", "adult": true, "has": ["pus"], "in": [], "on": ["your genitals"], "from": ["a prostitute","a hooker"], "is": ["a venereal disease","crotch rot"], "typeOf": ["a disease"], "supertypeOf": ["syphillis","chlamydia","herpes"], "nearlyIs": [], "property": [], "acts": ["itches"], "actsCont": ["an itching"], "recipient": ["cure","catch"], "recipientPast": []},</v>
@@ -24219,7 +24212,7 @@
         <v>1980</v>
       </c>
     </row>
-    <row r="193" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A193" t="str">
         <f t="shared" si="42"/>
         <v>{"spelling": "dye", "group": "_ie", "pos": "Noun", "adult": false, "has": ["a colour"], "in": [], "on": ["your hair"], "from": [], "is": [], "typeOf": ["a colouring"], "supertypeOf": [], "nearlyIs": ["a stain"], "property": ["a colourful"], "acts": ["colours","stains"], "actsCont": ["a colouring","a staining"], "recipient": [], "recipientPast": []},</v>
@@ -24313,7 +24306,7 @@
         <v>1883</v>
       </c>
     </row>
-    <row r="194" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A194" t="str">
         <f t="shared" si="42"/>
         <v>{"spelling": "guy", "group": "_ie", "pos": "Noun", "adult": false, "has": ["arms","legs","a body"], "in": [], "on": [], "from": [], "is": ["a man"], "typeOf": ["a person"], "supertypeOf": ["a boy","a lad"], "nearlyIs": [], "property": ["a masculine","a male"], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -24477,7 +24470,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="196" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A196" t="str">
         <f t="shared" si="42"/>
         <v>{"spelling": "lie", "group": "_ie", "pos": "Noun", "adult": false, "has": ["never happened"], "in": [], "on": [], "from": ["a politician","an advert","a conman"], "is": ["an untruth"], "typeOf": [], "supertypeOf": ["a deception"], "nearlyIs": [], "property": ["a deceitful"], "acts": ["deceives","misleads"], "actsCont": ["a deceiving","a misleading"], "recipient": [], "recipientPast": []},</v>
@@ -24577,7 +24570,7 @@
         <v>1988</v>
       </c>
     </row>
-    <row r="197" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A197" t="str">
         <f t="shared" si="42"/>
         <v>{"spelling": "eye", "group": "_ie", "pos": "Noun", "adult": false, "has": ["a pupil","a lens","lashes"], "in": [], "on": [], "from": [], "is": [], "typeOf": ["a body part"], "supertypeOf": [], "nearlyIs": ["a centre-point"], "property": [], "acts": ["sees","watches"], "actsCont": ["a seeing","a watching"], "recipient": ["blind"], "recipientPast": []},</v>
@@ -24674,7 +24667,7 @@
         <v>1993</v>
       </c>
     </row>
-    <row r="198" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A198" t="str">
         <f t="shared" si="42"/>
         <v>{"spelling": "bell", "group": "_ell", "pos": "Noun", "adult": false, "has": ["a clapper"], "in": ["a church","a steeple"], "on": [], "from": [], "is": [], "typeOf": ["an instrument"], "supertypeOf": [], "nearlyIs": ["a chime"], "property": [], "acts": ["rings","tolls"], "actsCont": ["a ringing","a tolling"], "recipient": ["ring","toll"], "recipientPast": []},</v>
@@ -24774,7 +24767,7 @@
         <v>1994</v>
       </c>
     </row>
-    <row r="199" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A199" t="str">
         <f t="shared" si="42"/>
         <v>{"spelling": "well", "group": "_ell", "pos": "Noun", "adult": false, "has": ["a bucket","water"], "in": [], "on": [], "from": [], "is": [], "typeOf": [], "supertypeOf": [], "nearlyIs": ["a resevoir"], "property": [], "acts": [], "actsCont": [], "recipient": ["dig","wish on"], "recipientPast": []},</v>
@@ -24856,7 +24849,7 @@
         <v>1999</v>
       </c>
     </row>
-    <row r="200" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A200" t="str">
         <f t="shared" si="42"/>
         <v>{"spelling": "yell", "group": "_ell", "pos": "Noun", "adult": false, "has": [], "in": [], "on": [], "from": ["a football fan","someone in trouble"], "is": ["a shout"], "typeOf": ["a noise","an exclamation"], "supertypeOf": ["a scream","a screech","a holler"], "nearlyIs": [], "property": ["a loud"], "acts": [], "actsCont": [], "recipient": ["shout","scream","hear"], "recipientPast": ["a shouted","a screamed"]},</v>
@@ -24965,7 +24958,7 @@
         <v>2003</v>
       </c>
     </row>
-    <row r="201" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A201" t="str">
         <f t="shared" si="42"/>
         <v>{"spelling": "shell", "group": "_ell", "pos": "Noun", "adult": false, "has": ["an inside"], "in": ["the sea","the ocean"], "on": ["the beach"], "from": ["an oyster","a clam"], "is": [], "typeOf": ["a casing","an exterior"], "supertypeOf": ["a conch"], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": ["launch"], "recipientPast": ["launched"]},</v>
@@ -25065,7 +25058,7 @@
         <v>2005</v>
       </c>
     </row>
-    <row r="202" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A202" t="str">
         <f t="shared" si="42"/>
         <v>{"spelling": "gel", "group": "_ell", "pos": "Noun", "adult": false, "has": [], "in": [], "on": [], "from": ["a bottle"], "is": [], "typeOf": [], "supertypeOf": ["a body-wash"], "nearlyIs": ["a liquid","a paste"], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -25144,7 +25137,7 @@
         <v>1325</v>
       </c>
     </row>
-    <row r="203" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A203" t="str">
         <f t="shared" si="42"/>
         <v>{"spelling": "hell", "group": "_ell", "pos": "Noun", "adult": true, "has": ["flames","sinners","pitchforks"], "in": [], "on": [], "from": [], "is": ["hades","an inferno"], "typeOf": ["a nightmare","an underworld","an afterlife"], "supertypeOf": [], "nearlyIs": [], "property": ["a burning","a nightmarish"], "acts": ["burns"], "actsCont": ["a burning"], "recipient": [], "recipientPast": []},</v>
@@ -25320,7 +25313,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="205" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A205" t="str">
         <f t="shared" si="42"/>
         <v>{"spelling": "smell", "group": "_ell", "pos": "Noun", "adult": false, "has": ["an origin"], "in": ["the bathroom","the toilet"], "on": [], "from": [], "is": ["an odour","an odor"], "typeOf": ["an emission"], "supertypeOf": ["a scent","a stench"], "nearlyIs": [], "property": ["a stinky"], "acts": ["stinks"], "actsCont": ["a stinking"], "recipient": [], "recipientPast": []},</v>
@@ -25420,7 +25413,7 @@
         <v>1878</v>
       </c>
     </row>
-    <row r="206" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A206" t="str">
         <f t="shared" si="42"/>
         <v>{"spelling": "act", "group": "_act", "pos": "Noun", "adult": false, "has": [], "in": ["a play"], "on": ["stage"], "from": [], "is": [], "typeOf": [], "supertypeOf": [], "nearlyIs": ["a chapter"], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -25566,7 +25559,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="208" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A208" t="str">
         <f t="shared" si="42"/>
         <v>{"spelling": "tact", "group": "_act", "pos": "Noun", "adult": false, "has": [], "in": [], "on": [], "from": ["a diplomat"], "is": [], "typeOf": ["manners"], "supertypeOf": [], "nearlyIs": ["a politeness"], "property": ["a careful"], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -25645,7 +25638,7 @@
         <v>1742</v>
       </c>
     </row>
-    <row r="209" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A209" t="str">
         <f t="shared" si="42"/>
         <v>{"spelling": "pact", "group": "_act", "pos": "Noun", "adult": false, "has": ["signatures"], "in": ["writing"], "on": [], "from": ["a diplomat"], "is": [], "typeOf": ["an agreement","a treaty"], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -25727,7 +25720,7 @@
         <v>1337</v>
       </c>
     </row>
-    <row r="210" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A210" t="str">
         <f t="shared" si="42"/>
         <v>{"spelling": "fact", "group": "_act", "pos": "Noun", "adult": false, "has": ["proof"], "in": [], "on": [], "from": [], "is": ["a truth"], "typeOf": [], "supertypeOf": [], "nearlyIs": [], "property": ["an objective"], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -25803,7 +25796,7 @@
         <v>1743</v>
       </c>
     </row>
-    <row r="211" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A211" t="str">
         <f t="shared" si="42"/>
         <v>{"spelling": "cough", "group": "_off", "pos": "Noun", "adult": false, "has": [], "in": [], "on": [], "from": ["a patient"], "is": [], "typeOf": ["a sound"], "supertypeOf": [], "nearlyIs": ["a hiccup"], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -25879,7 +25872,7 @@
         <v>1339</v>
       </c>
     </row>
-    <row r="212" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A212" t="str">
         <f t="shared" si="42"/>
         <v>{"spelling": "toff", "group": "_off", "pos": "Noun", "adult": false, "has": ["a tophat","riches","a monocle"], "in": ["the upper classes"], "on": [], "from": ["a rich family"], "is": ["a snob"], "typeOf": ["a gentleman"], "supertypeOf": [], "nearlyIs": [], "property": ["a posh"], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -25970,7 +25963,7 @@
         <v>1744</v>
       </c>
     </row>
-    <row r="213" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A213" t="str">
         <f t="shared" si="42"/>
         <v>{"spelling": "ride", "group": "_ide", "pos": "Noun", "adult": false, "has": ["tracks"], "in": ["a fairground","an amusement park"], "on": [], "from": [], "is": [], "typeOf": ["an attraction"], "supertypeOf": ["a rollercoaster","a log flume"], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -26055,7 +26048,7 @@
         <v>1343</v>
       </c>
     </row>
-    <row r="214" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A214" t="str">
         <f t="shared" si="42"/>
         <v>{"spelling": "tide", "group": "_ide", "pos": "Noun", "adult": false, "has": ["waves","a lot of water"], "in": ["the ocean"], "on": ["the beach"], "from": [], "is": [], "typeOf": [], "supertypeOf": [], "nearlyIs": ["a wave"], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -26207,7 +26200,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="216" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A216" t="str">
         <f t="shared" si="42"/>
         <v>{"spelling": "side", "group": "_ide", "pos": "Noun", "adult": false, "has": [], "in": [], "on": [], "from": [], "is": [], "typeOf": [], "supertypeOf": [], "nearlyIs": ["an edge"], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -26277,7 +26270,7 @@
         <v>1344</v>
       </c>
     </row>
-    <row r="217" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A217" t="str">
         <f t="shared" si="42"/>
         <v>{"spelling": "pride", "group": "_ide", "pos": "Noun", "adult": false, "has": ["lions"], "in": [], "on": [], "from": [], "is": [], "typeOf": [], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": ["inspire"], "recipientPast": []},</v>
@@ -26350,7 +26343,7 @@
         <v>2033</v>
       </c>
     </row>
-    <row r="218" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A218" t="str">
         <f t="shared" si="42"/>
         <v>{"spelling": "guide", "group": "_ide", "pos": "Noun", "adult": false, "has": ["expertise"], "in": [], "on": ["a hike","a tour"], "from": ["a gallery"], "is": [], "typeOf": ["a leader"], "supertypeOf": ["a guru"], "nearlyIs": [], "property": [], "acts": ["leads"], "actsCont": ["a leading"], "recipient": [], "recipientPast": []},</v>
@@ -26441,7 +26434,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="219" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A219" t="str">
         <f t="shared" si="42"/>
         <v>{"spelling": "hide", "group": "_ide", "pos": "Noun", "adult": false, "has": ["hunters"], "in": [], "on": ["an animal"], "from": [], "is": ["a pelt"], "typeOf": ["a covering","a skin"], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": ["skin"], "recipientPast": ["a skinned"]},</v>
@@ -26529,7 +26522,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="220" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A220" t="str">
         <f t="shared" si="42"/>
         <v>{"spelling": "child", "group": "_ild", "pos": "Noun", "adult": false, "has": ["parents"], "in": ["school","a classroom"], "on": [], "from": [], "is": ["a kid","a youth","a sprog"], "typeOf": ["a person"], "supertypeOf": ["a baby","a toddler","an urchin"], "nearlyIs": [], "property": ["a young"], "acts": ["plays"], "actsCont": ["a playing"], "recipient": ["teach"], "recipientPast": ["a taught"]},</v>
@@ -26641,7 +26634,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="221" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A221" t="str">
         <f t="shared" si="42"/>
         <v>{"spelling": "fin", "group": "_in", "pos": "Noun", "adult": false, "has": [], "in": [], "on": ["a fish"], "from": [], "is": [], "typeOf": [], "supertypeOf": ["a flipper"], "nearlyIs": ["a wing"], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -26717,7 +26710,7 @@
         <v>1354</v>
       </c>
     </row>
-    <row r="222" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A222" t="str">
         <f t="shared" si="42"/>
         <v>{"spelling": "win", "group": "_in", "pos": "Noun", "adult": false, "has": [], "in": ["sports"], "on": [], "from": [], "is": ["a victory"], "typeOf": ["a success"], "supertypeOf": [], "nearlyIs": [], "property": ["a victorious","a successful"], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -26799,7 +26792,7 @@
         <v>1674</v>
       </c>
     </row>
-    <row r="223" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A223" t="str">
         <f t="shared" si="42"/>
         <v>{"spelling": "tin", "group": "_in", "pos": "Noun", "adult": false, "has": ["a lid","a filling","an opener"], "in": ["the periodic table"], "on": ["the periodic table"], "from": [], "is": ["a can"], "typeOf": ["packaging"], "supertypeOf": [], "nearlyIs": [], "property": ["a metallic"], "acts": [], "actsCont": [], "recipient": ["open"], "recipientPast": []},</v>
@@ -26893,7 +26886,7 @@
         <v>1855</v>
       </c>
     </row>
-    <row r="224" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A224" t="str">
         <f t="shared" si="42"/>
         <v>{"spelling": "pin", "group": "_in", "pos": "Noun", "adult": false, "has": ["a head","a point"], "in": ["a pincushion","a voodoo doll"], "on": [], "from": [], "is": [], "typeOf": ["a spike","a fastening"], "supertypeOf": ["a tack","a thumbtack"], "nearlyIs": ["a needle"], "property": ["a sharp","a pointy"], "acts": ["punctures"], "actsCont": [], "recipient": ["stab with"], "recipientPast": []},</v>
@@ -26999,7 +26992,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="225" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A225" t="str">
         <f t="shared" si="42"/>
         <v>{"spelling": "sin", "group": "_in", "pos": "Noun", "adult": false, "has": [], "in": [], "on": [], "from": ["a sinner"], "is": [], "typeOf": [], "supertypeOf": ["murder","theft"], "nearlyIs": ["a crime"], "property": ["an immoral"], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -27081,7 +27074,7 @@
         <v>1749</v>
       </c>
     </row>
-    <row r="226" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A226" t="str">
         <f t="shared" si="42"/>
         <v>{"spelling": "din", "group": "_in", "pos": "Noun", "adult": false, "has": [], "in": [], "on": [], "from": ["a drumkit","an accordian","bagpipes"], "is": ["a cacophony"], "typeOf": ["a noise"], "supertypeOf": ["a clatter"], "nearlyIs": [], "property": ["a loud","a noisy"], "acts": [], "actsCont": [], "recipient": ["hear"], "recipientPast": []},</v>
@@ -27175,7 +27168,7 @@
         <v>1959</v>
       </c>
     </row>
-    <row r="227" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A227" t="str">
         <f t="shared" si="42"/>
         <v>{"spelling": "gin", "group": "_in", "pos": "Noun", "adult": false, "has": ["a lot of alcohol in it","juniper berries"], "in": ["a cocktail","a bar"], "on": [], "from": [], "is": [], "typeOf": ["a drink","a spirit","booze"], "supertypeOf": [], "nearlyIs": [], "property": ["an alcoholic"], "acts": [], "actsCont": [], "recipient": ["drink"], "recipientPast": []},</v>
@@ -27269,7 +27262,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="228" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A228" t="str">
         <f t="shared" si="42"/>
         <v>{"spelling": "djinn", "group": "_in", "pos": "Noun", "adult": false, "has": ["magical powers","a lamp"], "in": ["a lamp"], "on": [], "from": [], "is": ["a genie"], "typeOf": ["a spirit"], "supertypeOf": [], "nearlyIs": [], "property": ["a magical"], "acts": ["grants wishes"], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -27357,7 +27350,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="229" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A229" t="str">
         <f t="shared" si="42"/>
         <v>{"spelling": "kin", "group": "_in", "pos": "Noun", "adult": false, "has": [], "in": ["the family"], "on": [], "from": ["a family"], "is": ["a family member","a relative"], "typeOf": [], "supertypeOf": ["an aunt","an uncle","a cousin"], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -27445,7 +27438,7 @@
         <v>1376</v>
       </c>
     </row>
-    <row r="230" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A230" t="str">
         <f t="shared" si="42"/>
         <v>{"spelling": "bin", "group": "_in", "pos": "Noun", "adult": false, "has": ["a lid","rubbish"], "in": [], "on": [], "from": [], "is": [], "typeOf": [], "supertypeOf": ["a dumpster","a skip"], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -27524,7 +27517,7 @@
         <v>1378</v>
       </c>
     </row>
-    <row r="231" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A231" t="str">
         <f t="shared" si="42"/>
         <v>{"spelling": "shin", "group": "_in", "pos": "Noun", "adult": false, "has": ["a bone"], "in": ["your leg","your body"], "on": [], "from": [], "is": [], "typeOf": ["a body part","a bone"], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -27606,7 +27599,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="232" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A232" t="str">
         <f t="shared" si="42"/>
         <v>{"spelling": "chin", "group": "_in", "pos": "Noun", "adult": false, "has": ["a beard","a jaw"], "in": [], "on": ["your face"], "from": [], "is": [], "typeOf": ["a body part"], "supertypeOf": [], "nearlyIs": ["a jaw"], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -27688,7 +27681,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="233" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A233" t="str">
         <f t="shared" si="42"/>
         <v>{"spelling": "moat", "group": "_ote", "pos": "Noun", "adult": false, "has": ["a drawbridge"], "in": [], "on": [], "from": [], "is": [], "typeOf": ["a body of water"], "supertypeOf": [], "nearlyIs": ["a pond"], "property": ["a defensive"], "acts": [], "actsCont": [], "recipient": ["cross"], "recipientPast": []},</v>
@@ -27770,7 +27763,7 @@
         <v>1851</v>
       </c>
     </row>
-    <row r="234" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A234" t="str">
         <f t="shared" si="42"/>
         <v>{"spelling": "quote", "group": "_ote", "pos": "Noun", "adult": false, "has": ["been written down","an attribution"], "in": ["writing"], "on": [], "from": ["Shakespeare","an author","a guru"], "is": [], "typeOf": [], "supertypeOf": [], "nearlyIs": ["a saying"], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": ["a spoken","a written"]},</v>
@@ -27864,7 +27857,7 @@
         <v>1682</v>
       </c>
     </row>
-    <row r="235" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A235" t="str">
         <f t="shared" si="42"/>
         <v>{"spelling": "tote", "group": "_ote", "pos": "Noun", "adult": false, "has": ["a drawstring","clothes in it"], "in": [], "on": [], "from": [], "is": [], "typeOf": ["a bag"], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -27940,7 +27933,7 @@
         <v>1077</v>
       </c>
     </row>
-    <row r="236" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A236" t="str">
         <f t="shared" si="42"/>
         <v>{"spelling": "goat", "group": "_ote", "pos": "Noun", "adult": false, "has": ["horns","hooves"], "in": [], "on": [], "from": ["a farm","a farmyard"], "is": [], "typeOf": ["an animal","a farm animal","a mammal"], "supertypeOf": ["a kid"], "nearlyIs": ["a sheep"], "property": ["a horned"], "acts": ["bleats"], "actsCont": ["a bleating"], "recipient": [], "recipientPast": []},</v>
@@ -28043,7 +28036,7 @@
         <v>1881</v>
       </c>
     </row>
-    <row r="237" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A237" t="str">
         <f t="shared" si="42"/>
         <v>{"spelling": "vote", "group": "_ote", "pos": "Noun", "adult": false, "has": ["a party","political leanings"], "in": ["a ballot box"], "on": [], "from": [], "is": ["a ballot","a poll"], "typeOf": [], "supertypeOf": ["a secret ballot"], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": ["cast"], "recipientPast": ["a cast"]},</v>
@@ -28134,7 +28127,7 @@
         <v>1896</v>
       </c>
     </row>
-    <row r="238" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A238" t="str">
         <f t="shared" si="42"/>
         <v>{"spelling": "note", "group": "_ote", "pos": "Noun", "adult": false, "has": ["an author"], "in": [], "on": ["paper"], "from": ["a secret admirer"], "is": [], "typeOf": ["writing"], "supertypeOf": ["a memo"], "nearlyIs": ["a letter"], "property": ["a written"], "acts": [], "actsCont": [], "recipient": ["write","send"], "recipientPast": ["a written"]},</v>
@@ -28231,7 +28224,7 @@
         <v>1682</v>
       </c>
     </row>
-    <row r="239" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A239" t="str">
         <f t="shared" si="42"/>
         <v>{"spelling": "mote", "group": "_ote", "pos": "Noun", "adult": false, "has": [], "in": ["the air"], "on": [], "from": [], "is": [], "typeOf": [], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -28301,7 +28294,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="240" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A240" t="str">
         <f t="shared" si="42"/>
         <v>{"spelling": "stoat", "group": "_ote", "pos": "Noun", "adult": false, "has": ["whiskers","a tail"], "in": ["a burrow","the countryside"], "on": [], "from": [], "is": [], "typeOf": ["vermin","an animal","a mammal"], "supertypeOf": [], "nearlyIs": ["a ferret"], "property": ["a furry"], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -28465,7 +28458,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="242" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A242" t="str">
         <f t="shared" si="42"/>
         <v>{"spelling": "town", "group": "_own", "pos": "Noun", "adult": false, "has": ["inhabitants","buildings","a mayor"], "in": [], "on": [], "from": [], "is": [], "typeOf": ["a settlement"], "supertypeOf": [], "nearlyIs": ["a village","a city"], "property": ["a residential"], "acts": [], "actsCont": [], "recipient": ["live in","inhabit"], "recipientPast": ["an inhabited"]},</v>
@@ -28562,7 +28555,7 @@
         <v>2031</v>
       </c>
     </row>
-    <row r="243" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A243" t="str">
         <f t="shared" si="42"/>
         <v>{"spelling": "gown", "group": "_own", "pos": "Noun", "adult": false, "has": ["seams","material"], "in": ["a closet","a wardrobe"], "on": [], "from": [], "is": [], "typeOf": ["a garment","clothing"], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": ["wear"], "recipientPast": ["a worn"]},</v>
@@ -28653,7 +28646,7 @@
         <v>1886</v>
       </c>
     </row>
-    <row r="244" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A244" t="str">
         <f t="shared" si="42"/>
         <v>{"spelling": "sub", "group": "_ub", "pos": "Noun", "adult": false, "has": ["sailors","a periscope"], "in": ["the ocean","the sea"], "on": [], "from": [], "is": [], "typeOf": ["a boat","a ship","a vehicle"], "supertypeOf": [], "nearlyIs": [], "property": ["an underwater"], "acts": ["sails"], "actsCont": ["sailing"], "recipient": ["board","steer"], "recipientPast": []},</v>
@@ -28756,7 +28749,7 @@
         <v>2091</v>
       </c>
     </row>
-    <row r="245" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A245" t="str">
         <f t="shared" si="42"/>
         <v>{"spelling": "tub", "group": "_ub", "pos": "Noun", "adult": false, "has": [], "in": [], "on": [], "from": [], "is": ["a bath"], "typeOf": ["a container"], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -28829,7 +28822,7 @@
         <v>979</v>
       </c>
     </row>
-    <row r="246" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A246" t="str">
         <f t="shared" si="42"/>
         <v>{"spelling": "pub", "group": "_ub", "pos": "Noun", "adult": false, "has": ["drinks","beers","kegs"], "in": [], "on": [], "from": [], "is": ["a bar","a tavern"], "typeOf": [], "supertypeOf": [], "nearlyIs": ["a restaurant","a club","a microbrewery"], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -28920,7 +28913,7 @@
         <v>1484</v>
       </c>
     </row>
-    <row r="247" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A247" t="str">
         <f t="shared" si="42"/>
         <v>{"spelling": "hub", "group": "_ub", "pos": "Noun", "adult": false, "has": ["spokes"], "in": [], "on": [], "from": [], "is": ["a center"], "typeOf": [], "supertypeOf": [], "nearlyIs": [], "property": ["a central"], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -28996,7 +28989,7 @@
         <v>1782</v>
       </c>
     </row>
-    <row r="248" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A248" t="str">
         <f t="shared" si="42"/>
         <v>{"spelling": "law", "group": "_aw", "pos": "Noun", "adult": false, "has": ["rules"], "in": ["court"], "on": [], "from": [], "is": [], "typeOf": ["a rule"], "supertypeOf": [], "nearlyIs": [], "property": ["a legal"], "acts": [], "actsCont": [], "recipient": ["break"], "recipientPast": []},</v>
@@ -29078,7 +29071,7 @@
         <v>2032</v>
       </c>
     </row>
-    <row r="249" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A249" t="str">
         <f t="shared" si="42"/>
         <v>{"spelling": "awe", "group": "_aw", "pos": "Noun", "adult": false, "has": [], "in": [], "on": [], "from": [], "is": ["amazement"], "typeOf": [], "supertypeOf": [], "nearlyIs": ["worship"], "property": ["an amazing"], "acts": [], "actsCont": [], "recipient": ["inspire"], "recipientPast": []},</v>
@@ -29157,7 +29150,7 @@
         <v>2033</v>
       </c>
     </row>
-    <row r="250" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A250" t="str">
         <f t="shared" ref="A250:A313" si="56">CONCATENATE("{""spelling"": """,Q250,""", ""group"": """,O250,""", ""pos"": """,S250,""", ""adult"": ",IF(R250=TRUE,"true","false"),", ""has"": [",B250,"]",", ""in"": [",C250,"]",", ""on"": [",D250,"]",", ""from"": [",E250,"]",", ""is"": [",F250,"]",", ""typeOf"": [",G250,"]",", ""supertypeOf"": [",H250,"]",", ""nearlyIs"": [",I250,"]",", ""property"": [",J250,"]",", ""acts"": [",K250,"]",", ""actsCont"": [",L250,"]",", ""recipient"": [",M250,"]",", ""recipientPast"": [",N250,"]},")</f>
         <v>{"spelling": "paw", "group": "_aw", "pos": "Noun", "adult": false, "has": ["claws"], "in": [], "on": ["a dog's leg"], "from": [], "is": [], "typeOf": [], "supertypeOf": [], "nearlyIs": ["a hand"], "property": ["a clawed"], "acts": ["claws"], "actsCont": [], "recipient": ["declaw"], "recipientPast": []},</v>
@@ -29242,7 +29235,7 @@
         <v>2034</v>
       </c>
     </row>
-    <row r="251" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A251" t="str">
         <f t="shared" si="56"/>
         <v>{"spelling": "saw", "group": "_aw", "pos": "Noun", "adult": false, "has": ["teeth"], "in": ["a toolbox","a workshop"], "on": ["a workbench"], "from": [], "is": [], "typeOf": ["a tool"], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": ["cuts"], "actsCont": ["a cutting"], "recipient": ["sharpen"], "recipientPast": ["a sharpened"]},</v>
@@ -29336,7 +29329,7 @@
         <v>2038</v>
       </c>
     </row>
-    <row r="252" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A252" t="str">
         <f t="shared" si="56"/>
         <v>{"spelling": "jaw", "group": "_aw", "pos": "Noun", "adult": false, "has": ["teeth","bones"], "in": [], "on": ["a face"], "from": [], "is": [], "typeOf": [], "supertypeOf": [], "nearlyIs": ["a mouth","a chin"], "property": [], "acts": ["chews"], "actsCont": ["a chewing"], "recipient": [], "recipientPast": []},</v>
@@ -29424,7 +29417,7 @@
         <v>2040</v>
       </c>
     </row>
-    <row r="253" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A253" t="str">
         <f t="shared" si="56"/>
         <v>{"spelling": "caw", "group": "_aw", "pos": "Noun", "adult": false, "has": [], "in": [], "on": [], "from": ["a raven","a crow","a blackbird"], "is": [], "typeOf": ["a noise","a birdcall"], "supertypeOf": [], "nearlyIs": ["a squawk"], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -29509,7 +29502,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="254" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A254" t="str">
         <f t="shared" si="56"/>
         <v>{"spelling": "maw", "group": "_aw", "pos": "Noun", "adult": false, "has": ["teeth","a tongue"], "in": [], "on": [], "from": [], "is": [], "typeOf": ["a mouth"], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": ["chews","swallows","eat"], "actsCont": ["a chewing","a swallowing","an eating"], "recipient": [], "recipientPast": []},</v>
@@ -29603,7 +29596,7 @@
         <v>2043</v>
       </c>
     </row>
-    <row r="255" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A255" t="str">
         <f t="shared" si="56"/>
         <v>{"spelling": "call", "group": "_all", "pos": "Noun", "adult": false, "has": [], "in": [], "on": [], "from": [], "is": [], "typeOf": ["a noise","a request"], "supertypeOf": [], "nearlyIs": ["a shout"], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -29679,7 +29672,7 @@
         <v>1193</v>
       </c>
     </row>
-    <row r="256" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A256" t="str">
         <f t="shared" si="56"/>
         <v>{"spelling": "wall", "group": "_all", "pos": "Noun", "adult": false, "has": ["bricks","mortar"], "in": [], "on": [], "from": [], "is": [], "typeOf": [], "supertypeOf": ["a fence"], "nearlyIs": [], "property": ["a brick"], "acts": [], "actsCont": [], "recipient": ["build","demolish"], "recipientPast": ["a built"]},</v>
@@ -29767,7 +29760,7 @@
         <v>2045</v>
       </c>
     </row>
-    <row r="257" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A257" t="str">
         <f t="shared" si="56"/>
         <v>{"spelling": "drawl", "group": "_all", "pos": "Noun", "adult": false, "has": ["an accent"], "in": [], "on": [], "from": [], "is": [], "typeOf": ["an accent"], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -29840,7 +29833,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="258" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A258" t="str">
         <f t="shared" si="56"/>
         <v>{"spelling": "hall", "group": "_all", "pos": "Noun", "adult": false, "has": ["rooms"], "in": ["a house","a mansion"], "on": [], "from": [], "is": [], "typeOf": ["a room"], "supertypeOf": ["a throne-room"], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -29922,7 +29915,7 @@
         <v>1409</v>
       </c>
     </row>
-    <row r="259" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A259" t="str">
         <f t="shared" si="56"/>
         <v>{"spelling": "ball", "group": "_all", "pos": "Noun", "adult": false, "has": [], "in": [], "on": ["a pitch","a stadium"], "from": ["a bowler","a pitcher"], "is": [], "typeOf": ["a sphere"], "supertypeOf": [], "nearlyIs": [], "property": ["a round","a spherical"], "acts": ["bounces"], "actsCont": ["a bouncing"], "recipient": ["throw","catch"], "recipientPast": ["a thrown","a caught"]},</v>
@@ -30028,7 +30021,7 @@
         <v>2049</v>
       </c>
     </row>
-    <row r="260" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A260" t="str">
         <f t="shared" si="56"/>
         <v>{"spelling": "maul", "group": "_all", "pos": "Noun", "adult": false, "has": [], "in": ["an arsenal"], "on": [], "from": [], "is": [], "typeOf": ["a hammer","a weapon","a club"], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": ["swing"], "recipientPast": []},</v>
@@ -30110,7 +30103,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="261" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A261" t="str">
         <f t="shared" si="56"/>
         <v>{"spelling": "shawl", "group": "_all", "pos": "Noun", "adult": false, "has": ["fabric"], "in": [], "on": ["an old lady"], "from": [], "is": [], "typeOf": ["clothing","a garment"], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": ["wear"], "recipientPast": ["a worn"]},</v>
@@ -30195,7 +30188,7 @@
         <v>1886</v>
       </c>
     </row>
-    <row r="262" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A262" t="str">
         <f t="shared" si="56"/>
         <v>{"spelling": "man", "group": "_an", "pos": "Noun", "adult": false, "has": ["arms","legs","a body"], "in": [], "on": [], "from": ["Mars"], "is": [], "typeOf": ["a person"], "supertypeOf": ["a boy","a chap","a gent"], "nearlyIs": [], "property": ["a male","a masculine"], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -30292,7 +30285,7 @@
         <v>1735</v>
       </c>
     </row>
-    <row r="263" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A263" t="str">
         <f t="shared" si="56"/>
         <v>{"spelling": "tan", "group": "_an", "pos": "Noun", "adult": false, "has": ["skin","freckles"], "in": [], "on": [], "from": ["holiday","vacation"], "is": [], "typeOf": ["a colouration","a colour"], "supertypeOf": [], "nearlyIs": [], "property": ["a brown"], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -30380,7 +30373,7 @@
         <v>1764</v>
       </c>
     </row>
-    <row r="264" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A264" t="str">
         <f t="shared" si="56"/>
         <v>{"spelling": "pan", "group": "_an", "pos": "Noun", "adult": false, "has": ["a handle"], "in": ["the kitchen","a kitchen"], "on": ["the stove"], "from": [], "is": [], "typeOf": [], "supertypeOf": ["a wok"], "nearlyIs": ["a pot"], "property": [], "acts": [], "actsCont": [], "recipient": ["cook with"], "recipientPast": []},</v>
@@ -30468,7 +30461,7 @@
         <v>1812</v>
       </c>
     </row>
-    <row r="265" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A265" t="str">
         <f t="shared" si="56"/>
         <v>{"spelling": "fan", "group": "_an", "pos": "Noun", "adult": false, "has": ["blades"], "in": ["the summer"], "on": [], "from": [], "is": [], "typeOf": ["an appliance"], "supertypeOf": [], "nearlyIs": ["an air conditioner"], "property": [], "acts": ["spins","blows"], "actsCont": ["a spinning","a blowing"], "recipient": [], "recipientPast": []},</v>
@@ -30559,7 +30552,7 @@
         <v>2054</v>
       </c>
     </row>
-    <row r="266" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A266" t="str">
         <f t="shared" si="56"/>
         <v>{"spelling": "can", "group": "_an", "pos": "Noun", "adult": false, "has": ["a lid","an opener","a filling"], "in": ["the pantry"], "on": [], "from": [], "is": ["a tin"], "typeOf": ["packaging"], "supertypeOf": [], "nearlyIs": [], "property": ["a tin"], "acts": [], "actsCont": [], "recipient": ["open"], "recipientPast": []},</v>
@@ -30650,7 +30643,7 @@
         <v>1855</v>
       </c>
     </row>
-    <row r="267" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A267" t="str">
         <f t="shared" si="56"/>
         <v>{"spelling": "ban", "group": "_an", "pos": "Noun", "adult": false, "has": [], "in": [], "on": [], "from": [], "is": [], "typeOf": ["a restriction","a law","a rule"], "supertypeOf": [], "nearlyIs": [], "property": ["a forbidden"], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -30729,7 +30722,7 @@
         <v>1765</v>
       </c>
     </row>
-    <row r="268" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A268" t="str">
         <f t="shared" si="56"/>
         <v>{"spelling": "nan", "group": "_an", "pos": "Noun", "adult": false, "has": ["grandchildren","grandkids"], "in": [], "on": [], "from": [], "is": ["a grandma","a grandmother"], "typeOf": ["a grandparent","a relative","a woman"], "supertypeOf": [], "nearlyIs": [], "property": ["an elderly"], "acts": ["knits"], "actsCont": ["a knitting"], "recipient": [], "recipientPast": []},</v>
@@ -30826,7 +30819,7 @@
         <v>2056</v>
       </c>
     </row>
-    <row r="269" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A269" t="str">
         <f t="shared" si="56"/>
         <v>{"spelling": "dog", "group": "_og", "pos": "Noun", "adult": false, "has": ["a tail","paws","a collar"], "in": ["a kennel","the pound"], "on": [], "from": ["the pound"], "is": ["a hound"], "typeOf": ["a pet","an animal","a mammal"], "supertypeOf": ["a pup","a puppy"], "nearlyIs": [], "property": ["a fluffy"], "acts": ["barks","woofs"], "actsCont": ["a barking","a woofing"], "recipient": ["play with","feed","walk"], "recipientPast": []},</v>
@@ -30953,7 +30946,7 @@
         <v>1826</v>
       </c>
     </row>
-    <row r="270" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A270" t="str">
         <f t="shared" si="56"/>
         <v>{"spelling": "fog", "group": "_og", "pos": "Noun", "adult": false, "has": [], "in": [], "on": [], "from": [], "is": ["a mist"], "typeOf": [], "supertypeOf": ["a smog"], "nearlyIs": ["a cloud"], "property": ["a misty"], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -31032,7 +31025,7 @@
         <v>1767</v>
       </c>
     </row>
-    <row r="271" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A271" t="str">
         <f t="shared" si="56"/>
         <v>{"spelling": "hog", "group": "_og", "pos": "Noun", "adult": false, "has": ["a snout","a curly tail","bristles"], "in": ["a sty","a farmyard","a farm"], "on": [], "from": ["a farmyard","a farm"], "is": ["a pig"], "typeOf": ["an animal","a farm animal","a mammal"], "supertypeOf": ["a piglet","a boar"], "nearlyIs": [], "property": [], "acts": ["oinks"], "actsCont": ["an oinking"], "recipient": [], "recipientPast": []},</v>
@@ -31147,7 +31140,7 @@
         <v>2060</v>
       </c>
     </row>
-    <row r="272" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A272" t="str">
         <f t="shared" si="56"/>
         <v>{"spelling": "jog", "group": "_og", "pos": "Noun", "adult": false, "has": [], "in": [], "on": [], "from": [], "is": ["a run"], "typeOf": [], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -31217,7 +31210,7 @@
         <v>1430</v>
       </c>
     </row>
-    <row r="273" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A273" t="str">
         <f t="shared" si="56"/>
         <v>{"spelling": "log", "group": "_og", "pos": "Noun", "adult": false, "has": ["rings","bark"], "in": ["a fireplace","a bonfire"], "on": ["a bonfire","a fire"], "from": ["a woodcutter","a lumberjack"], "is": [], "typeOf": ["wood","firewood"], "supertypeOf": [], "nearlyIs": ["a plank"], "property": ["a wooden"], "acts": [], "actsCont": [], "recipient": ["saw","burn"], "recipientPast": ["a sawn"]},</v>
@@ -31329,7 +31322,7 @@
         <v>2062</v>
       </c>
     </row>
-    <row r="274" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A274" t="str">
         <f t="shared" si="56"/>
         <v>{"spelling": "cog", "group": "_og", "pos": "Noun", "adult": false, "has": ["teeth"], "in": ["a clock","a machine"], "on": [], "from": [], "is": ["a gear"], "typeOf": ["a wheel","a mechanism"], "supertypeOf": [], "nearlyIs": [], "property": ["a mechanical"], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -31417,7 +31410,7 @@
         <v>1769</v>
       </c>
     </row>
-    <row r="275" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A275" t="str">
         <f t="shared" si="56"/>
         <v>{"spelling": "bog", "group": "_og", "pos": "Noun", "adult": false, "has": ["reeds","mosquitos","crocodiles"], "in": [], "on": [], "from": [], "is": ["a swamp","a mire"], "typeOf": [], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -31499,7 +31492,7 @@
         <v>1438</v>
       </c>
     </row>
-    <row r="276" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A276" t="str">
         <f t="shared" si="56"/>
         <v>{"spelling": "cub", "group": "_ub", "pos": "Noun", "adult": false, "has": ["claws","fur"], "in": ["the woods"], "on": [], "from": [], "is": [], "typeOf": ["a bear","a lion","a wolf"], "supertypeOf": [], "nearlyIs": [], "property": ["a young","a furry"], "acts": ["howls"], "actsCont": ["a howling"], "recipient": [], "recipientPast": []},</v>
@@ -31596,7 +31589,7 @@
         <v>2093</v>
       </c>
     </row>
-    <row r="277" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A277" t="str">
         <f t="shared" si="56"/>
         <v>{"spelling": "blog", "group": "_og", "pos": "Noun", "adult": false, "has": ["articles","pictures"], "in": [], "on": ["the internet","Wordpress","Tumblr"], "from": [], "is": [], "typeOf": [], "supertypeOf": [], "nearlyIs": [], "property": ["an online","a digital","a written"], "acts": [], "actsCont": [], "recipient": ["write","post","read"], "recipientPast": ["a written","a posted","a read"]},</v>
@@ -31705,7 +31698,7 @@
         <v>2066</v>
       </c>
     </row>
-    <row r="278" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A278" t="str">
         <f t="shared" si="56"/>
         <v>{"spelling": "sprog", "group": "_og", "pos": "Noun", "adult": false, "has": ["parents","a diaper","a dummy"], "in": ["diapers","school","kindergarten"], "on": [], "from": [], "is": ["a child","a kid","a youth"], "typeOf": ["a person"], "supertypeOf": ["a baby","a toddler","an urchin"], "nearlyIs": [], "property": ["a young"], "acts": ["cries"], "actsCont": ["a crying"], "recipient": ["change","feed","burp"], "recipientPast": []},</v>
@@ -31829,7 +31822,7 @@
         <v>2070</v>
       </c>
     </row>
-    <row r="279" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A279" t="str">
         <f t="shared" si="56"/>
         <v>{"spelling": "slog", "group": "_og", "pos": "Noun", "adult": false, "has": [], "in": [], "on": [], "from": [], "is": ["a drudgery"], "typeOf": ["a hardship"], "supertypeOf": [], "nearlyIs": [], "property": ["a tough"], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -31905,7 +31898,7 @@
         <v>1771</v>
       </c>
     </row>
-    <row r="280" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A280" t="str">
         <f t="shared" si="56"/>
         <v>{"spelling": "snog", "group": "_og", "pos": "Noun", "adult": false, "has": ["tongues"], "in": [], "on": [], "from": ["two lovers"], "is": [], "typeOf": ["a kiss"], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -31981,7 +31974,7 @@
         <v>1442</v>
       </c>
     </row>
-    <row r="281" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A281" t="str">
         <f t="shared" si="56"/>
         <v>{"spelling": "smog", "group": "_og", "pos": "Noun", "adult": false, "has": [], "in": [], "on": [], "from": ["a chimney","a factory"], "is": [], "typeOf": ["a fog"], "supertypeOf": [], "nearlyIs": [], "property": ["a polluted"], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -32060,7 +32053,7 @@
         <v>1772</v>
       </c>
     </row>
-    <row r="282" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A282" t="str">
         <f t="shared" si="56"/>
         <v>{"spelling": "club", "group": "_ub", "pos": "Noun", "adult": false, "has": ["drinks","music","a DJ"], "in": [], "on": [], "from": [], "is": ["a bar"], "typeOf": ["a weapon"], "supertypeOf": ["a mace","a maul","a hammer"], "nearlyIs": [], "property": ["a blunt"], "acts": [], "actsCont": [], "recipient": ["swing"], "recipientPast": []},</v>
@@ -32157,7 +32150,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="283" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A283" t="str">
         <f t="shared" si="56"/>
         <v>{"spelling": "stub", "group": "_ub", "pos": "Noun", "adult": false, "has": [], "in": [], "on": [], "from": [], "is": ["a butt"], "typeOf": ["an end"], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -32230,7 +32223,7 @@
         <v>1493</v>
       </c>
     </row>
-    <row r="284" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A284" t="str">
         <f t="shared" si="56"/>
         <v>{"spelling": "nub", "group": "_ub", "pos": "Noun", "adult": false, "has": [], "in": [], "on": [], "from": [], "is": [], "typeOf": ["a lump"], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -32300,7 +32293,7 @@
         <v>1495</v>
       </c>
     </row>
-    <row r="285" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A285" t="str">
         <f t="shared" si="56"/>
         <v>{"spelling": "duck", "group": "_uck", "pos": "Noun", "adult": false, "has": ["feathers","a beak","wings"], "in": ["the river","a river"], "on": [], "from": [], "is": [], "typeOf": ["a bird","an animal"], "supertypeOf": ["a mallard"], "nearlyIs": [], "property": ["a feathered"], "acts": ["flies","quacks"], "actsCont": ["a flying","a quacking"], "recipient": ["eat"], "recipientPast": []},</v>
@@ -32409,7 +32402,7 @@
         <v>1861</v>
       </c>
     </row>
-    <row r="286" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A286" t="str">
         <f t="shared" si="56"/>
         <v>{"spelling": "puck", "group": "_uck", "pos": "Noun", "adult": false, "has": [], "in": ["a hockey match"], "on": ["an ice rink"], "from": [], "is": [], "typeOf": [], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": ["hit"], "recipientPast": []},</v>
@@ -32485,7 +32478,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="287" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A287" t="str">
         <f t="shared" si="56"/>
         <v>{"spelling": "fuck", "group": "_uck", "pos": "Noun", "adult": true, "has": ["foreplay","a climax","an orgasm"], "in": [], "on": ["tinder"], "from": ["tinder","a prostitute","a hooker"], "is": ["a shag","a lay","a sexual partner"], "typeOf": [], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -32585,7 +32578,7 @@
         <v>1278</v>
       </c>
     </row>
-    <row r="288" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A288" t="str">
         <f t="shared" si="56"/>
         <v>{"spelling": "luck", "group": "_uck", "pos": "Noun", "adult": false, "has": [], "in": [], "on": [], "from": [], "is": ["chance"], "typeOf": [], "supertypeOf": ["fortune","misfortune"], "nearlyIs": [], "property": ["a flukey","a risky"], "acts": ["runs out"], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -32670,7 +32663,7 @@
         <v>1975</v>
       </c>
     </row>
-    <row r="289" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A289" t="str">
         <f t="shared" si="56"/>
         <v>{"spelling": "cook", "group": "_uck", "pos": "Noun", "adult": false, "has": ["ingredients","knives","a kitchen"], "in": ["the kitchen","a kitchen","a restaurant"], "on": [], "from": [], "is": ["a chef"], "typeOf": [], "supertypeOf": ["a baker"], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -32761,7 +32754,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="290" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A290" t="str">
         <f t="shared" si="56"/>
         <v>{"spelling": "buck", "group": "_uck", "pos": "Noun", "adult": false, "has": ["antlers","hooves"], "in": ["the woods","a tip jar"], "on": [], "from": [], "is": ["a dollar"], "typeOf": ["a deer","an animal","a wild animal"], "supertypeOf": [], "nearlyIs": [], "property": ["a horned"], "acts": [], "actsCont": [], "recipient": ["spend"], "recipientPast": []},</v>
@@ -32858,7 +32851,7 @@
         <v>1976</v>
       </c>
     </row>
-    <row r="291" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A291" t="str">
         <f t="shared" si="56"/>
         <v>{"spelling": "muck", "group": "_uck", "pos": "Noun", "adult": false, "has": [], "in": ["a farmyard","a field"], "on": ["the bottom of your shoe"], "from": [], "is": ["dirt"], "typeOf": ["a stain"], "supertypeOf": [], "nearlyIs": ["rubbish"], "property": ["a dirty"], "acts": [], "actsCont": [], "recipient": ["clean up"], "recipientPast": []},</v>
@@ -32949,7 +32942,7 @@
         <v>1945</v>
       </c>
     </row>
-    <row r="292" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A292" t="str">
         <f t="shared" si="56"/>
         <v>{"spelling": "mum", "group": "_um", "pos": "Noun", "adult": false, "has": ["a child","kids"], "in": [], "on": [], "from": [], "is": ["a mother"], "typeOf": ["a parent"], "supertypeOf": [], "nearlyIs": [], "property": ["a maternal","a parental"], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -33034,7 +33027,7 @@
         <v>1755</v>
       </c>
     </row>
-    <row r="293" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A293" t="str">
         <f t="shared" si="56"/>
         <v>{"spelling": "bum", "group": "_um", "pos": "Noun", "adult": false, "has": ["cheeks"], "in": ["your pants"], "on": [], "from": [], "is": ["a tramp"], "typeOf": ["a body part","a rear"], "supertypeOf": [], "nearlyIs": ["a seat"], "property": [], "acts": ["farts","poops"], "actsCont": ["a farting","a pooping"], "recipient": ["wipe"], "recipientPast": ["a wiped"]},</v>
@@ -33137,7 +33130,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="294" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A294" t="str">
         <f t="shared" si="56"/>
         <v>{"spelling": "sum", "group": "_um", "pos": "Noun", "adult": false, "has": ["numbers","an answer"], "in": [], "on": [], "from": [], "is": ["a total"], "typeOf": ["an equation"], "supertypeOf": [], "nearlyIs": [], "property": ["a mathematical","a total"], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -33222,7 +33215,7 @@
         <v>1389</v>
       </c>
     </row>
-    <row r="295" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A295" t="str">
         <f t="shared" si="56"/>
         <v>{"spelling": "gum", "group": "_um", "pos": "Noun", "adult": false, "has": [], "in": [], "on": ["the bottom of your shoe"], "from": [], "is": [], "typeOf": [], "supertypeOf": [], "nearlyIs": [], "property": ["a chewy"], "acts": [], "actsCont": [], "recipient": ["chew"], "recipientPast": ["a chewed"]},</v>
@@ -33301,7 +33294,7 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="296" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A296" t="str">
         <f t="shared" si="56"/>
         <v>{"spelling": "egg", "group": "_eg", "pos": "Noun", "adult": false, "has": ["a yolk","a shell"], "in": ["a carton","an omlette"], "on": ["toast"], "from": ["a chicken","a farm"], "is": [], "typeOf": ["a food","an ingredient"], "supertypeOf": [], "nearlyIs": [], "property": ["a round","a fragile"], "acts": ["hatches"], "actsCont": ["a hatching"], "recipient": ["eat","crack","lay"], "recipientPast": ["a laid"]},</v>
@@ -33419,7 +33412,7 @@
         <v>2085</v>
       </c>
     </row>
-    <row r="297" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A297" t="str">
         <f t="shared" si="56"/>
         <v>{"spelling": "leg", "group": "_eg", "pos": "Noun", "adult": false, "has": ["a foot","a knee","a shin"], "in": [], "on": [], "from": [], "is": [], "typeOf": ["a limb","a body part"], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -33501,7 +33494,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="298" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A298" t="str">
         <f t="shared" si="56"/>
         <v>{"spelling": "peg", "group": "_eg", "pos": "Noun", "adult": false, "has": [], "in": [], "on": ["a washing line"], "from": [], "is": [], "typeOf": [], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -33571,7 +33564,7 @@
         <v>907</v>
       </c>
     </row>
-    <row r="299" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A299" t="str">
         <f t="shared" si="56"/>
         <v>{"spelling": "keg", "group": "_eg", "pos": "Noun", "adult": false, "has": ["beer","ale"], "in": ["a brewery","a pub","a bar"], "on": [], "from": ["a brewery"], "is": ["a cask"], "typeOf": ["a container"], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": ["tap"], "recipientPast": ["a tapped"]},</v>
@@ -33668,7 +33661,7 @@
         <v>2086</v>
       </c>
     </row>
-    <row r="300" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A300" t="str">
         <f t="shared" si="56"/>
         <v>{"spelling": "pass", "group": "_ass", "pos": "Noun", "adult": false, "has": [], "in": [], "on": [], "from": [], "is": [], "typeOf": ["a gap"], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -33738,7 +33731,7 @@
         <v>1462</v>
       </c>
     </row>
-    <row r="301" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A301" t="str">
         <f t="shared" si="56"/>
         <v>{"spelling": "gas", "group": "_ass", "pos": "Noun", "adult": false, "has": ["a smell"], "in": ["a canister"], "on": [], "from": ["a fart"], "is": [], "typeOf": [], "supertypeOf": ["a fart","a vapour"], "nearlyIs": [], "property": [], "acts": ["smells","stinks"], "actsCont": ["a stinking"], "recipient": ["smell"], "recipientPast": []},</v>
@@ -33832,7 +33825,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="302" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A302" t="str">
         <f t="shared" si="56"/>
         <v>{"spelling": "lass", "group": "_ass", "pos": "Noun", "adult": false, "has": ["a skirt"], "in": ["a dress","a skirt","pigtails"], "on": [], "from": [], "is": ["a girl"], "typeOf": ["a woman"], "supertypeOf": [], "nearlyIs": ["a lady"], "property": ["a female","a feminine"], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -33926,7 +33919,7 @@
         <v>1654</v>
       </c>
     </row>
-    <row r="303" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A303" t="str">
         <f t="shared" si="56"/>
         <v>{"spelling": "mass", "group": "_ass", "pos": "Noun", "adult": false, "has": ["weight"], "in": [], "on": [], "from": [], "is": ["a weight"], "typeOf": [], "supertypeOf": [], "nearlyIs": [], "property": ["a large"], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -34002,7 +33995,7 @@
         <v>1663</v>
       </c>
     </row>
-    <row r="304" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A304" t="str">
         <f t="shared" si="56"/>
         <v>{"spelling": "port", "group": "_ort", "pos": "Noun", "adult": false, "has": ["ships","boats","yachts"], "in": [], "on": ["the coast"], "from": [], "is": ["a harbour"], "typeOf": [], "supertypeOf": [], "nearlyIs": ["a cove"], "property": [], "acts": [], "actsCont": [], "recipient": ["sail into"], "recipientPast": []},</v>
@@ -34090,7 +34083,7 @@
         <v>1971</v>
       </c>
     </row>
-    <row r="305" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A305" t="str">
         <f t="shared" si="56"/>
         <v>{"spelling": "wart", "group": "_ort", "pos": "Noun", "adult": false, "has": [], "in": [], "on": [], "from": [], "is": [], "typeOf": ["a blemish"], "supertypeOf": [], "nearlyIs": ["a mole","a spot"], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -34166,7 +34159,7 @@
         <v>1032</v>
       </c>
     </row>
-    <row r="306" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A306" t="str">
         <f t="shared" si="56"/>
         <v>{"spelling": "fort", "group": "_ort", "pos": "Noun", "adult": false, "has": ["a drawbridge","walls","towers"], "in": ["a castle"], "on": [], "from": [], "is": ["a keep","a castle"], "typeOf": [], "supertypeOf": [], "nearlyIs": ["a guardpost"], "property": ["a defensive","a defensible","a fortified"], "acts": ["protects"], "actsCont": [], "recipient": ["invade","seige"], "recipientPast": ["a beseiged"]},</v>
@@ -34275,7 +34268,7 @@
         <v>2090</v>
       </c>
     </row>
-    <row r="307" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A307" t="str">
         <f t="shared" si="56"/>
         <v>{"spelling": "court", "group": "_ort", "pos": "Noun", "adult": false, "has": ["judges","lawyers"], "in": [], "on": [], "from": [], "is": [], "typeOf": [], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -34348,7 +34341,7 @@
         <v>932</v>
       </c>
     </row>
-    <row r="308" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A308" t="str">
         <f t="shared" si="56"/>
         <v>{"spelling": "cum", "group": "_um", "pos": "Noun", "adult": true, "has": [], "in": ["a condom"], "on": [], "from": ["your dick","your cock"], "is": ["spunk","jizz","sperm"], "typeOf": ["an emission"], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -34439,7 +34432,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="309" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A309" t="str">
         <f t="shared" si="56"/>
         <v>{"spelling": "pun", "group": "_un", "pos": "Noun", "adult": false, "has": ["a setup","a punchline"], "in": [], "on": [], "from": [], "is": [], "typeOf": ["a joke","a riddle"], "supertypeOf": [], "nearlyIs": [], "property": ["a funny","a hilarious"], "acts": [], "actsCont": [], "recipient": ["tell"], "recipientPast": []},</v>
@@ -34527,7 +34520,7 @@
         <v>1989</v>
       </c>
     </row>
-    <row r="310" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A310" t="str">
         <f t="shared" si="56"/>
         <v>{"spelling": "ton", "group": "_un", "pos": "Noun", "adult": false, "has": ["a lot in it"], "in": [], "on": [], "from": [], "is": [], "typeOf": ["a weight"], "supertypeOf": [], "nearlyIs": ["a lot"], "property": ["a heavy","a weighty"], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -34679,7 +34672,7 @@
         <v>1504</v>
       </c>
     </row>
-    <row r="312" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A312" t="str">
         <f t="shared" si="56"/>
         <v>{"spelling": "sun", "group": "_un", "pos": "Noun", "adult": false, "has": ["rays","light"], "in": ["space","the sky"], "on": [], "from": [], "is": [], "typeOf": ["a star"], "supertypeOf": [], "nearlyIs": [], "property": ["a bright","a stellar"], "acts": ["burns","shines"], "actsCont": ["a burning","a shining"], "recipient": [], "recipientPast": []},</v>
@@ -34779,7 +34772,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="313" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A313" t="str">
         <f t="shared" si="56"/>
         <v>{"spelling": "bun", "group": "_un", "pos": "Noun", "adult": false, "has": ["currants","dough"], "in": ["the oven"], "on": [], "from": ["the bakery","a baker"], "is": [], "typeOf": ["a bread","a bakery product"], "supertypeOf": ["a bap","a roll"], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": ["eat","bake"], "recipientPast": ["a baked"]},</v>
@@ -34884,7 +34877,7 @@
     </row>
     <row r="314" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
       <c r="A314" t="str">
-        <f t="shared" ref="A314:A377" si="70">CONCATENATE("{""spelling"": """,Q314,""", ""group"": """,O314,""", ""pos"": """,S314,""", ""adult"": ",IF(R314=TRUE,"true","false"),", ""has"": [",B314,"]",", ""in"": [",C314,"]",", ""on"": [",D314,"]",", ""from"": [",E314,"]",", ""is"": [",F314,"]",", ""typeOf"": [",G314,"]",", ""supertypeOf"": [",H314,"]",", ""nearlyIs"": [",I314,"]",", ""property"": [",J314,"]",", ""acts"": [",K314,"]",", ""actsCont"": [",L314,"]",", ""recipient"": [",M314,"]",", ""recipientPast"": [",N314,"]},")</f>
+        <f t="shared" ref="A314:A333" si="70">CONCATENATE("{""spelling"": """,Q314,""", ""group"": """,O314,""", ""pos"": """,S314,""", ""adult"": ",IF(R314=TRUE,"true","false"),", ""has"": [",B314,"]",", ""in"": [",C314,"]",", ""on"": [",D314,"]",", ""from"": [",E314,"]",", ""is"": [",F314,"]",", ""typeOf"": [",G314,"]",", ""supertypeOf"": [",H314,"]",", ""nearlyIs"": [",I314,"]",", ""property"": [",J314,"]",", ""acts"": [",K314,"]",", ""actsCont"": [",L314,"]",", ""recipient"": [",M314,"]",", ""recipientPast"": [",N314,"]},")</f>
         <v>{"spelling": "up", "group": "_up", "pos": "Adj", "adult": false, "has": [], "in": [], "on": [], "from": [], "is": [], "typeOf": [], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
       </c>
       <c r="B314" t="str">
@@ -34952,7 +34945,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="315" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A315" t="str">
         <f t="shared" si="70"/>
         <v>{"spelling": "pup", "group": "_up", "pos": "Noun", "adult": false, "has": ["a tail","paws"], "in": ["a kennel"], "on": [], "from": [], "is": [], "typeOf": ["a dog","a pet","an animal"], "supertypeOf": [], "nearlyIs": [], "property": ["a fluffy","a canine"], "acts": ["barks","yaps"], "actsCont": ["a barking","a yapping"], "recipient": ["play with","feed","walk"], "recipientPast": []},</v>
@@ -35064,7 +35057,7 @@
         <v>1826</v>
       </c>
     </row>
-    <row r="316" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A316" t="str">
         <f t="shared" si="70"/>
         <v>{"spelling": "cup", "group": "_up", "pos": "Noun", "adult": false, "has": ["a handle","a saucer"], "in": [], "on": [], "from": [], "is": ["a mug"], "typeOf": ["china"], "supertypeOf": [], "nearlyIs": ["a glass"], "property": [], "acts": [], "actsCont": [], "recipient": ["drink from"], "recipientPast": []},</v>
@@ -35149,7 +35142,7 @@
         <v>2029</v>
       </c>
     </row>
-    <row r="317" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A317" t="str">
         <f t="shared" si="70"/>
         <v>{"spelling": "war", "group": "_aw", "pos": "Noun", "adult": false, "has": ["armies","combatants","an opponent"], "in": [], "on": ["campaign"], "from": [], "is": [], "typeOf": ["a conflict","combat"], "supertypeOf": ["a battle","an engagement"], "nearlyIs": ["a fight"], "property": [], "acts": ["kills"], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -35246,7 +35239,7 @@
         <v>2094</v>
       </c>
     </row>
-    <row r="318" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A318" t="str">
         <f t="shared" si="70"/>
         <v>{"spelling": "yore", "group": "_aw", "pos": "Noun", "adult": false, "has": [], "in": ["the past"], "on": [], "from": [], "is": [], "typeOf": [], "supertypeOf": [], "nearlyIs": [], "property": ["a historic","an ancient"], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -35322,7 +35315,7 @@
         <v>1785</v>
       </c>
     </row>
-    <row r="319" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A319" t="str">
         <f t="shared" si="70"/>
         <v>{"spelling": "pour", "group": "_aw", "pos": "Noun", "adult": false, "has": ["a liquid"], "in": ["a bar","a pub"], "on": [], "from": [], "is": [], "typeOf": ["a measure"], "supertypeOf": ["a shot","a jigger"], "nearlyIs": ["a drink"], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -35410,7 +35403,7 @@
         <v>1368</v>
       </c>
     </row>
-    <row r="320" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A320" t="str">
         <f t="shared" si="70"/>
         <v>{"spelling": "door", "group": "_aw", "pos": "Noun", "adult": false, "has": ["a handle","a bell"], "in": ["a house","a hallway"], "on": [], "from": [], "is": [], "typeOf": [], "supertypeOf": ["a gate"], "nearlyIs": [], "property": ["an open","a closed"], "acts": ["opens","closes","slams"], "actsCont": ["an opening","a closing"], "recipient": ["open","close","slam"], "recipientPast": []},</v>
@@ -35522,7 +35515,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="321" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A321" t="str">
         <f t="shared" si="70"/>
         <v>{"spelling": "gore", "group": "_aw", "pos": "Noun", "adult": true, "has": ["blood","bones"], "in": ["battle","war","a murder"], "on": [], "from": ["a victim"], "is": [], "typeOf": ["someone's remains"], "supertypeOf": [], "nearlyIs": ["offal"], "property": ["a vicious","a bloody"], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -35692,7 +35685,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="323" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A323" t="str">
         <f t="shared" si="70"/>
         <v>{"spelling": "whore", "group": "_aw", "pos": "Noun", "adult": true, "has": ["a pimp","fishnets"], "in": ["a dark alley","a brothel"], "on": ["the streets","a street corner"], "from": ["a brothel"], "is": ["a prostitute","a ho","a hooker"], "typeOf": [], "supertypeOf": [], "nearlyIs": [], "property": ["a slutty","a skanky"], "acts": ["shags","sucks","fucks"], "actsCont": ["a shagging","a fucking"], "recipient": ["shag","fuck","sleep with"], "recipientPast": []},</v>
@@ -35822,7 +35815,7 @@
         <v>1911</v>
       </c>
     </row>
-    <row r="324" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A324" t="str">
         <f t="shared" si="70"/>
         <v>{"spelling": "bore", "group": "_aw", "pos": "Noun", "adult": false, "has": ["no friends","no conversation"], "in": [], "on": [], "from": [], "is": [], "typeOf": [], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": ["drill"], "recipientPast": ["a drilled"]},</v>
@@ -35901,7 +35894,7 @@
         <v>2101</v>
       </c>
     </row>
-    <row r="325" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A325" t="str">
         <f t="shared" si="70"/>
         <v>{"spelling": "fish", "group": "_ish", "pos": "Noun", "adult": false, "has": ["scales","fins","gills"], "in": ["the sea","the ocean","a pond"], "on": [], "from": [], "is": [], "typeOf": ["an animal","an aquatic animal"], "supertypeOf": ["a shark","a salmon","a tuna"], "nearlyIs": ["sealife"], "property": ["a scaly","an underwater"], "acts": ["swims"], "actsCont": ["a swimming"], "recipient": ["catch","eat"], "recipientPast": []},</v>
@@ -36022,7 +36015,7 @@
         <v>1861</v>
       </c>
     </row>
-    <row r="326" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A326" t="str">
         <f t="shared" si="70"/>
         <v>{"spelling": "wish", "group": "_ish", "pos": "Noun", "adult": false, "has": [], "in": [], "on": [], "from": ["a genie","a fairy godmother"], "is": [], "typeOf": ["a desire","a want","a craving"], "supertypeOf": [], "nearlyIs": ["a hope"], "property": [], "acts": ["comes true"], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -36110,7 +36103,7 @@
         <v>2104</v>
       </c>
     </row>
-    <row r="327" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A327" t="str">
         <f t="shared" si="70"/>
         <v>{"spelling": "dish", "group": "_ish", "pos": "Noun", "adult": false, "has": [], "in": ["a kitchen","a cupboard"], "on": [], "from": [], "is": [], "typeOf": ["china","a platter"], "supertypeOf": [], "nearlyIs": ["a plate","a bowl"], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -36195,7 +36188,7 @@
         <v>1539</v>
       </c>
     </row>
-    <row r="328" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A328" t="str">
         <f t="shared" si="70"/>
         <v>{"spelling": "trooper", "group": "_uper", "pos": "Noun", "adult": false, "has": ["a gun","a uniform"], "in": ["the army","the police"], "on": ["patrol"], "from": [], "is": [], "typeOf": ["a soldier","a police officer"], "supertypeOf": [], "nearlyIs": ["an officer"], "property": [], "acts": ["patrols"], "actsCont": ["a patrolling"], "recipient": [], "recipientPast": []},</v>
@@ -36292,7 +36285,7 @@
         <v>2106</v>
       </c>
     </row>
-    <row r="329" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A329" t="str">
         <f t="shared" si="70"/>
         <v>{"spelling": "duper", "group": "_uper", "pos": "Noun", "adult": false, "has": ["no morals"], "in": [], "on": [], "from": [], "is": ["a liar"], "typeOf": [], "supertypeOf": ["a con","a conman"], "nearlyIs": ["a lawyer","a politician","a trickster"], "property": ["a deceitful"], "acts": ["lies","deceives"], "actsCont": ["a lying","a deceiving"], "recipient": [], "recipientPast": []},</v>
@@ -36395,7 +36388,7 @@
         <v>1985</v>
       </c>
     </row>
-    <row r="330" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A330" t="str">
         <f t="shared" si="70"/>
         <v>{"spelling": "cooper", "group": "_uper", "pos": "Noun", "adult": false, "has": ["tools","barrels"], "in": [], "on": [], "from": [], "is": ["a barrel maker"], "typeOf": ["a craftsman","an artisan"], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -36477,7 +36470,7 @@
         <v>1561</v>
       </c>
     </row>
-    <row r="331" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A331" t="str">
         <f t="shared" si="70"/>
         <v>{"spelling": "blooper", "group": "_uper", "pos": "Noun", "adult": false, "has": ["mistakes"], "in": [], "on": ["tv","a DVD"], "from": ["a movie","a film"], "is": ["an outtake"], "typeOf": ["a mistake"], "supertypeOf": [], "nearlyIs": [], "property": ["an accidental"], "acts": [], "actsCont": [], "recipient": ["watch","laugh at"], "recipientPast": ["a watched"]},</v>
@@ -36577,7 +36570,7 @@
         <v>1924</v>
       </c>
     </row>
-    <row r="332" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A332" t="str">
         <f t="shared" si="70"/>
         <v>{"spelling": "snooper", "group": "_uper", "pos": "Noun", "adult": false, "has": [], "in": [], "on": [], "from": [], "is": ["an investigator"], "typeOf": [], "supertypeOf": ["a paparazzi","a detective"], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -36653,7 +36646,7 @@
         <v>1570</v>
       </c>
     </row>
-    <row r="333" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A333" t="str">
         <f t="shared" si="70"/>
         <v>{"spelling": "trouper", "group": "_uper", "pos": "Noun", "adult": false, "has": [], "in": [], "on": [], "from": [], "is": ["an actor"], "typeOf": ["an entertainer"], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": ["acts","sings","performs"], "actsCont": ["an acting","a singing","a performing"], "recipient": [], "recipientPast": []},</v>
@@ -36744,7 +36737,7 @@
         <v>2113</v>
       </c>
     </row>
-    <row r="334" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A334" t="str">
         <f t="shared" ref="A334:A346" si="84">CONCATENATE("{""spelling"": """,Q334,""", ""group"": """,O334,""", ""pos"": """,S334,""", ""adult"": ",IF(R334=TRUE,"true","false"),", ""has"": [",B334,"]",", ""in"": [",C334,"]",", ""on"": [",D334,"]",", ""from"": [",E334,"]",", ""is"": [",F334,"]",", ""typeOf"": [",G334,"]",", ""supertypeOf"": [",H334,"]",", ""nearlyIs"": [",I334,"]",", ""property"": [",J334,"]",", ""acts"": [",K334,"]",", ""actsCont"": [",L334,"]",", ""recipient"": [",M334,"]",", ""recipientPast"": [",N334,"]},")</f>
         <v>{"spelling": "line", "group": "_ine", "pos": "Noun", "adult": false, "has": ["a start point","an end point","a gradient"], "in": ["a drawing"], "on": [], "from": [], "is": ["a queue"], "typeOf": ["a shape"], "supertypeOf": ["a tangent","an intersection"], "nearlyIs": ["a stroke"], "property": ["a straight"], "acts": [], "actsCont": [], "recipient": ["draw"], "recipientPast": ["a drawn"]},</v>
@@ -36847,7 +36840,7 @@
         <v>1900</v>
       </c>
     </row>
-    <row r="335" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A335" t="str">
         <f t="shared" si="84"/>
         <v>{"spelling": "wine", "group": "_ine", "pos": "Noun", "adult": false, "has": ["alcohol","tannins"], "in": ["a bottle","a glass","a cask"], "on": [], "from": ["a bottle","a cask"], "is": [], "typeOf": ["alcohol","a beverage","a drink"], "supertypeOf": ["a merlot","a chardonnay","a pinot noir"], "nearlyIs": ["champagne"], "property": ["an alcoholic"], "acts": [], "actsCont": [], "recipient": ["drink","bottle"], "recipientPast": ["a bottled"]},</v>
@@ -36968,7 +36961,7 @@
         <v>2115</v>
       </c>
     </row>
-    <row r="336" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A336" t="str">
         <f t="shared" si="84"/>
         <v>{"spelling": "pine", "group": "_ine", "pos": "Noun", "adult": false, "has": ["leaves","needles","bark"], "in": ["a forest","a wood","the woods"], "on": [], "from": [], "is": [], "typeOf": ["a tree","an evergreen"], "supertypeOf": ["a fir"], "nearlyIs": [], "property": ["an evergreen"], "acts": [], "actsCont": [], "recipient": ["chop down"], "recipientPast": []},</v>
@@ -37068,7 +37061,7 @@
         <v>1808</v>
       </c>
     </row>
-    <row r="337" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A337" t="str">
         <f t="shared" si="84"/>
         <v>{"spelling": "sign", "group": "_ine", "pos": "Noun", "adult": false, "has": ["a post","instructions"], "in": [], "on": ["a street"], "from": [], "is": [], "typeOf": ["a mark","a pointer"], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": ["read"], "recipientPast": []},</v>
@@ -37153,7 +37146,7 @@
         <v>2065</v>
       </c>
     </row>
-    <row r="338" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A338" t="str">
         <f t="shared" si="84"/>
         <v>{"spelling": "fine", "group": "_ine", "pos": "Noun", "adult": false, "has": ["a cost"], "in": [], "on": [], "from": ["a court","a police officer","a judge"], "is": ["a fee"], "typeOf": ["a punishment","a charge"], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": ["pay"], "recipientPast": []},</v>
@@ -37244,7 +37237,7 @@
         <v>2116</v>
       </c>
     </row>
-    <row r="339" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A339" t="str">
         <f t="shared" si="84"/>
         <v>{"spelling": "vine", "group": "_ine", "pos": "Noun", "adult": false, "has": ["grapes","leaves","a stem"], "in": ["a field"], "on": ["a wall","a trellis"], "from": [], "is": [], "typeOf": ["a plant"], "supertypeOf": ["a grape"], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -37335,7 +37328,7 @@
         <v>1611</v>
       </c>
     </row>
-    <row r="340" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A340" t="str">
         <f t="shared" si="84"/>
         <v>{"spelling": "mine", "group": "_ine", "pos": "Noun", "adult": false, "has": ["diamonds","a detonator","gold"], "in": ["the mountains"], "on": ["a battlefield"], "from": [], "is": [], "typeOf": ["a pit","an explosive","a bomb"], "supertypeOf": ["a quarry"], "nearlyIs": ["a tripwire"], "property": [], "acts": ["explodes"], "actsCont": [], "recipient": ["lay","dig","excavate"], "recipientPast": ["a laid","an excavated"]},</v>
@@ -37520,7 +37513,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="342" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A342" t="str">
         <f t="shared" si="84"/>
         <v>{"spelling": "top", "group": "_op", "pos": "Noun", "adult": false, "has": [], "in": [], "on": [], "from": [], "is": [], "typeOf": ["a direction","a side"], "supertypeOf": ["a peak","a summit"], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -37599,7 +37592,7 @@
         <v>1630</v>
       </c>
     </row>
-    <row r="343" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A343" t="str">
         <f t="shared" si="84"/>
         <v>{"spelling": "fop", "group": "_op", "pos": "Noun", "adult": false, "has": ["elaborate clothes"], "in": [], "on": [], "from": [], "is": ["a dandy"], "typeOf": ["a poser"], "supertypeOf": [], "nearlyIs": ["a toff"], "property": ["a posh","a well-dressed"], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
@@ -37684,7 +37677,7 @@
         <v>1793</v>
       </c>
     </row>
-    <row r="344" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A344" t="str">
         <f t="shared" si="84"/>
         <v>{"spelling": "hop", "group": "_op", "pos": "Noun", "adult": false, "has": [], "in": [], "on": [], "from": ["a rabbit","a kangaroo"], "is": [], "typeOf": ["a jump","a movement","a bounce"], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": ["brew"], "recipientPast": []},</v>
@@ -37769,7 +37762,7 @@
         <v>2120</v>
       </c>
     </row>
-    <row r="345" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A345" t="str">
         <f t="shared" si="84"/>
         <v>{"spelling": "cop", "group": "_op", "pos": "Noun", "adult": false, "has": ["a uniform","a badge","handcuffs"], "in": ["the police force"], "on": [], "from": [], "is": ["a police officer"], "typeOf": [], "supertypeOf": ["a trooper"], "nearlyIs": [], "property": [], "acts": ["patrols"], "actsCont": ["a patrolling"], "recipient": [], "recipientPast": []},</v>
@@ -37860,7 +37853,7 @@
         <v>2106</v>
       </c>
     </row>
-    <row r="346" spans="1:57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A346" t="str">
         <f t="shared" si="84"/>
         <v>{"spelling": "mop", "group": "_op", "pos": "Noun", "adult": false, "has": ["a handle"], "in": ["a cleaning trolley"], "on": [], "from": [], "is": [], "typeOf": [], "supertypeOf": ["a tool","a cleaning product"], "nearlyIs": ["a broom"], "property": [], "acts": ["cleans"], "actsCont": ["a cleaning"], "recipient": [], "recipientPast": []},</v>

</xml_diff>